<commit_message>
073 STEW TAYLOR data fix
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -1034,9 +1034,7 @@
       <c r="E8" s="12">
         <v>38.0</v>
       </c>
-      <c r="F8" s="13">
-        <v>29.0</v>
-      </c>
+      <c r="F8" s="13"/>
       <c r="G8" s="12">
         <v>32.0</v>
       </c>
@@ -1061,7 +1059,7 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>164</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
074 Week 6/5 data update
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="75">
   <si>
     <t>WINTER GOLF 25/26 - THURSDAY SINGLES</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>30th Oct 25</t>
+  </si>
+  <si>
+    <t>6th Nov 25</t>
   </si>
   <si>
     <t>NAME</t>
@@ -174,6 +177,9 @@
   </si>
   <si>
     <t>2nd Nov 25</t>
+  </si>
+  <si>
+    <t>9th Nov 25</t>
   </si>
   <si>
     <t>MICK SKINNER</t>
@@ -801,7 +807,9 @@
       <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="4"/>
+      <c r="H3" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="4"/>
       <c r="K3" s="3"/>
@@ -824,87 +832,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13">
@@ -917,7 +925,9 @@
         <v>19.0</v>
       </c>
       <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
+      <c r="H5" s="13">
+        <v>35.0</v>
+      </c>
       <c r="I5" s="12"/>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
@@ -938,12 +948,12 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>87</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" s="12">
         <v>28.0</v>
@@ -958,7 +968,9 @@
       <c r="G6" s="12">
         <v>33.0</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="13">
+        <v>32.0</v>
+      </c>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
       <c r="K6" s="15"/>
@@ -979,12 +991,12 @@
       <c r="Z6" s="18"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="12">
         <v>31.0</v>
@@ -997,7 +1009,9 @@
       </c>
       <c r="F7" s="13"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="13"/>
+      <c r="H7" s="13">
+        <v>41.0</v>
+      </c>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
       <c r="K7" s="15"/>
@@ -1018,12 +1032,12 @@
       <c r="Z7" s="18"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>103</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="12">
         <v>31.0</v>
@@ -1038,7 +1052,9 @@
       <c r="G8" s="12">
         <v>32.0</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="13">
+        <v>38.0</v>
+      </c>
       <c r="I8" s="12"/>
       <c r="J8" s="13"/>
       <c r="K8" s="15"/>
@@ -1059,12 +1075,12 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="12">
         <v>34.0</v>
@@ -1081,7 +1097,9 @@
       <c r="G9" s="12">
         <v>30.0</v>
       </c>
-      <c r="H9" s="13"/>
+      <c r="H9" s="13">
+        <v>35.0</v>
+      </c>
       <c r="I9" s="15"/>
       <c r="J9" s="14"/>
       <c r="K9" s="15"/>
@@ -1102,12 +1120,12 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>156</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="12">
         <v>21.0</v>
@@ -1116,7 +1134,9 @@
       <c r="E10" s="12"/>
       <c r="F10" s="14"/>
       <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="13">
+        <v>31.0</v>
+      </c>
       <c r="I10" s="12"/>
       <c r="J10" s="13"/>
       <c r="K10" s="15"/>
@@ -1137,12 +1157,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="12">
         <v>36.0</v>
@@ -1159,7 +1179,9 @@
       <c r="G11" s="12">
         <v>15.0</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="13">
+        <v>32.0</v>
+      </c>
       <c r="I11" s="12"/>
       <c r="J11" s="14"/>
       <c r="K11" s="15"/>
@@ -1180,12 +1202,12 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>143</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C12" s="12">
         <v>35.0</v>
@@ -1200,7 +1222,9 @@
       <c r="G12" s="12">
         <v>30.0</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="13">
+        <v>36.0</v>
+      </c>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
       <c r="K12" s="15"/>
@@ -1221,12 +1245,12 @@
       <c r="Z12" s="18"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>129</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C13" s="12">
         <v>34.0</v>
@@ -1237,7 +1261,9 @@
       <c r="G13" s="12">
         <v>22.0</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="13">
+        <v>30.0</v>
+      </c>
       <c r="I13" s="15"/>
       <c r="J13" s="14"/>
       <c r="K13" s="15"/>
@@ -1258,12 +1284,12 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C14" s="12">
         <v>33.0</v>
@@ -1278,7 +1304,9 @@
       <c r="G14" s="12">
         <v>34.0</v>
       </c>
-      <c r="H14" s="14"/>
+      <c r="H14" s="13">
+        <v>36.0</v>
+      </c>
       <c r="I14" s="12"/>
       <c r="J14" s="13"/>
       <c r="K14" s="12"/>
@@ -1299,12 +1327,12 @@
       <c r="Z14" s="18"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>127</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -1337,7 +1365,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
@@ -1350,7 +1378,9 @@
       <c r="G16" s="12">
         <v>36.0</v>
       </c>
-      <c r="H16" s="14"/>
+      <c r="H16" s="13">
+        <v>34.0</v>
+      </c>
       <c r="I16" s="12"/>
       <c r="J16" s="13"/>
       <c r="K16" s="15"/>
@@ -1371,12 +1401,12 @@
       <c r="Z16" s="18"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>94</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" s="18">
         <v>26.0</v>
@@ -1387,7 +1417,9 @@
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="12"/>
-      <c r="H17" s="13"/>
+      <c r="H17" s="13">
+        <v>32.0</v>
+      </c>
       <c r="I17" s="12"/>
       <c r="J17" s="13"/>
       <c r="K17" s="15"/>
@@ -1408,12 +1440,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C18" s="12">
         <v>31.0</v>
@@ -1426,7 +1458,9 @@
       <c r="G18" s="12">
         <v>35.0</v>
       </c>
-      <c r="H18" s="15"/>
+      <c r="H18" s="12">
+        <v>28.0</v>
+      </c>
       <c r="I18" s="12"/>
       <c r="J18" s="15"/>
       <c r="K18" s="12"/>
@@ -1447,7 +1481,7 @@
       <c r="Z18" s="12"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -1478,24 +1512,26 @@
     </row>
     <row r="20" ht="72.0" customHeight="1">
       <c r="B20" s="23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E20" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="H20" s="24"/>
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
@@ -1518,7 +1554,7 @@
     </row>
     <row r="21">
       <c r="B21" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C21" s="27">
         <v>36.0</v>
@@ -1535,7 +1571,9 @@
       <c r="G21" s="27">
         <v>36.0</v>
       </c>
-      <c r="H21" s="27"/>
+      <c r="H21" s="27">
+        <v>41.0</v>
+      </c>
       <c r="I21" s="27"/>
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
@@ -1578,25 +1616,27 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>54</v>
+      </c>
       <c r="H3" s="3"/>
       <c r="I3" s="4"/>
       <c r="J3" s="3"/>
@@ -1620,87 +1660,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
@@ -1708,7 +1748,9 @@
         <v>24.0</v>
       </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="12"/>
+      <c r="G5" s="12">
+        <v>26.0</v>
+      </c>
       <c r="H5" s="14"/>
       <c r="I5" s="12"/>
       <c r="J5" s="13"/>
@@ -1730,12 +1772,12 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA22" si="1">SUM(C5:Z5)</f>
-        <v>24</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" s="12">
         <v>38.0</v>
@@ -1745,7 +1787,9 @@
         <v>38.0</v>
       </c>
       <c r="F6" s="13"/>
-      <c r="G6" s="12"/>
+      <c r="G6" s="12">
+        <v>37.0</v>
+      </c>
       <c r="H6" s="13"/>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
@@ -1767,12 +1811,12 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>76</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
@@ -1784,7 +1828,9 @@
       <c r="F7" s="13">
         <v>24.0</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="12">
+        <v>43.0</v>
+      </c>
       <c r="H7" s="13"/>
       <c r="I7" s="12"/>
       <c r="J7" s="14"/>
@@ -1806,12 +1852,12 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C8" s="12">
         <v>28.0</v>
@@ -1823,7 +1869,9 @@
       <c r="F8" s="13">
         <v>24.0</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="12">
+        <v>36.0</v>
+      </c>
       <c r="H8" s="13"/>
       <c r="I8" s="12"/>
       <c r="J8" s="13"/>
@@ -1845,12 +1893,12 @@
       <c r="Z8" s="18"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13">
@@ -1860,7 +1908,9 @@
         <v>39.0</v>
       </c>
       <c r="F9" s="13"/>
-      <c r="G9" s="12"/>
+      <c r="G9" s="12">
+        <v>33.0</v>
+      </c>
       <c r="H9" s="13"/>
       <c r="I9" s="15"/>
       <c r="J9" s="14"/>
@@ -1882,12 +1932,12 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
@@ -1922,7 +1972,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C11" s="12">
         <v>33.0</v>
@@ -1934,7 +1984,9 @@
       <c r="F11" s="13">
         <v>34.0</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="12">
+        <v>37.0</v>
+      </c>
       <c r="H11" s="14"/>
       <c r="I11" s="15"/>
       <c r="J11" s="14"/>
@@ -1956,12 +2008,12 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>104</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -1969,7 +2021,9 @@
       <c r="F12" s="13">
         <v>30.0</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="12">
+        <v>33.0</v>
+      </c>
       <c r="H12" s="13"/>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
@@ -1991,12 +2045,12 @@
       <c r="Z12" s="18"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C13" s="12">
         <v>33.0</v>
@@ -2006,7 +2060,9 @@
       <c r="F13" s="13">
         <v>23.0</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="12">
+        <v>26.0</v>
+      </c>
       <c r="H13" s="13"/>
       <c r="I13" s="15"/>
       <c r="J13" s="13"/>
@@ -2028,12 +2084,12 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14" s="12">
         <v>29.0</v>
@@ -2045,7 +2101,9 @@
       <c r="F14" s="13">
         <v>27.0</v>
       </c>
-      <c r="G14" s="12"/>
+      <c r="G14" s="12">
+        <v>31.0</v>
+      </c>
       <c r="H14" s="14"/>
       <c r="I14" s="15"/>
       <c r="J14" s="13"/>
@@ -2067,12 +2125,12 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>81</v>
+        <v>112</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C15" s="12">
         <v>28.0</v>
@@ -2086,7 +2144,9 @@
       <c r="F15" s="13">
         <v>29.0</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="12">
+        <v>34.0</v>
+      </c>
       <c r="H15" s="14"/>
       <c r="I15" s="15"/>
       <c r="J15" s="14"/>
@@ -2108,12 +2168,12 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>110</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" s="12">
         <v>24.0</v>
@@ -2125,7 +2185,9 @@
       <c r="F16" s="13">
         <v>32.0</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="12">
+        <v>35.0</v>
+      </c>
       <c r="H16" s="13"/>
       <c r="I16" s="15"/>
       <c r="J16" s="14"/>
@@ -2147,12 +2209,12 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>87</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C17" s="12">
         <v>31.0</v>
@@ -2164,7 +2226,9 @@
         <v>27.0</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="G17" s="12"/>
+      <c r="G17" s="12">
+        <v>29.0</v>
+      </c>
       <c r="H17" s="13"/>
       <c r="I17" s="12"/>
       <c r="J17" s="13"/>
@@ -2186,12 +2250,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>97</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C18" s="12">
         <v>35.0</v>
@@ -2203,7 +2267,9 @@
         <v>34.0</v>
       </c>
       <c r="F18" s="13"/>
-      <c r="G18" s="12"/>
+      <c r="G18" s="12">
+        <v>31.0</v>
+      </c>
       <c r="H18" s="13"/>
       <c r="I18" s="12"/>
       <c r="J18" s="13"/>
@@ -2225,12 +2291,12 @@
       <c r="Z18" s="18"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>102</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C19" s="12">
         <v>33.0</v>
@@ -2242,7 +2308,9 @@
       <c r="F19" s="13">
         <v>29.0</v>
       </c>
-      <c r="G19" s="12"/>
+      <c r="G19" s="12">
+        <v>37.0</v>
+      </c>
       <c r="H19" s="13"/>
       <c r="I19" s="12"/>
       <c r="J19" s="13"/>
@@ -2264,12 +2332,12 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>99</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C20" s="12">
         <v>27.0</v>
@@ -2304,7 +2372,7 @@
     </row>
     <row r="21">
       <c r="B21" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C21" s="12">
         <v>31.0</v>
@@ -2343,7 +2411,7 @@
     </row>
     <row r="22">
       <c r="B22" s="28" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
@@ -2351,7 +2419,9 @@
         <v>33.0</v>
       </c>
       <c r="F22" s="13"/>
-      <c r="G22" s="12"/>
+      <c r="G22" s="12">
+        <v>32.0</v>
+      </c>
       <c r="H22" s="13"/>
       <c r="I22" s="12"/>
       <c r="J22" s="13"/>
@@ -2373,7 +2443,7 @@
       <c r="Z22" s="18"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -2404,21 +2474,23 @@
     </row>
     <row r="24" ht="84.75" customHeight="1">
       <c r="B24" s="23" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="G24" s="24"/>
+        <v>40</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>44</v>
+      </c>
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
       <c r="J24" s="24"/>
@@ -2442,7 +2514,7 @@
     </row>
     <row r="25">
       <c r="B25" s="26" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C25" s="27">
         <v>38.0</v>
@@ -2456,7 +2528,9 @@
       <c r="F25" s="27">
         <v>35.0</v>
       </c>
-      <c r="G25" s="27"/>
+      <c r="G25" s="27">
+        <v>43.0</v>
+      </c>
       <c r="H25" s="27"/>
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
@@ -2500,18 +2574,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -2520,7 +2594,7 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -2529,7 +2603,7 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -2538,7 +2612,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -2547,16 +2621,16 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
-        <v>19.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -2565,7 +2639,7 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -2574,7 +2648,7 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -2583,7 +2657,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -2592,7 +2666,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -2601,7 +2675,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34">
@@ -2610,7 +2684,7 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -2619,7 +2693,7 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -2628,34 +2702,34 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
-        <v>22.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="34">
@@ -2664,7 +2738,7 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="34">
@@ -2673,7 +2747,7 @@
     </row>
     <row r="20">
       <c r="A20" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="34">
@@ -2682,7 +2756,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="34">
@@ -2691,7 +2765,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="34">
@@ -2700,7 +2774,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="34">
@@ -2709,7 +2783,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B24" s="36"/>
       <c r="C24" s="37">
@@ -2718,7 +2792,7 @@
     </row>
     <row r="25">
       <c r="A25" s="35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="13">
@@ -6631,13 +6705,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2">
@@ -6645,10 +6719,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -6656,10 +6730,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4">
@@ -6667,10 +6741,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
@@ -6678,19 +6752,21 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="13">
         <v>5.0</v>
       </c>
-      <c r="B6" s="43"/>
+      <c r="B6" s="43" t="s">
+        <v>36</v>
+      </c>
       <c r="C6" s="44" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7">
@@ -6698,7 +6774,9 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="43"/>
-      <c r="C7" s="44"/>
+      <c r="C7" s="44" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="13">
@@ -11704,19 +11782,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
@@ -11809,11 +11887,11 @@
       </c>
       <c r="B6" s="46" t="str">
         <f>'SUNDAY SINGLES'!G24</f>
-        <v/>
-      </c>
-      <c r="C6" s="46" t="str">
+        <v>LES DOBBINS</v>
+      </c>
+      <c r="C6" s="46">
         <f>'SUNDAY SINGLES'!G25</f>
-        <v/>
+        <v>43</v>
       </c>
       <c r="D6" s="47" t="str">
         <f>'THURSDAY SINGLES'!G20</f>
@@ -11838,11 +11916,11 @@
       </c>
       <c r="D7" s="47" t="str">
         <f>'THURSDAY SINGLES'!H20</f>
-        <v/>
-      </c>
-      <c r="E7" s="46" t="str">
+        <v>MARTIN BROCK</v>
+      </c>
+      <c r="E7" s="46">
         <f>'THURSDAY SINGLES'!H21</f>
-        <v/>
+        <v>41</v>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Week 7/6 data update
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="79">
   <si>
     <t>WINTER GOLF 25/26 - THURSDAY SINGLES</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>6th Nov 25</t>
+  </si>
+  <si>
+    <t>13th  Nov 25</t>
   </si>
   <si>
     <t>NAME</t>
@@ -182,6 +185,9 @@
     <t>9th Nov 25</t>
   </si>
   <si>
+    <t>16th Nov 25</t>
+  </si>
+  <si>
     <t>MICK SKINNER</t>
   </si>
   <si>
@@ -212,6 +218,9 @@
     <t>ARTHUR YOUNG</t>
   </si>
   <si>
+    <t>GAZ LENTON</t>
+  </si>
+  <si>
     <t>WHITE TEES</t>
   </si>
   <si>
@@ -228,6 +237,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>PAUL HANCOX</t>
   </si>
   <si>
     <t>SUNDAY</t>
@@ -810,7 +822,9 @@
       <c r="H3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="3"/>
+      <c r="I3" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="J3" s="4"/>
       <c r="K3" s="3"/>
       <c r="L3" s="4"/>
@@ -832,87 +846,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13">
@@ -928,7 +942,9 @@
       <c r="H5" s="13">
         <v>35.0</v>
       </c>
-      <c r="I5" s="12"/>
+      <c r="I5" s="12">
+        <v>40.0</v>
+      </c>
       <c r="J5" s="14"/>
       <c r="K5" s="15"/>
       <c r="L5" s="14"/>
@@ -948,12 +964,12 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>122</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="12">
         <v>28.0</v>
@@ -996,7 +1012,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C7" s="12">
         <v>31.0</v>
@@ -1012,7 +1028,9 @@
       <c r="H7" s="13">
         <v>41.0</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="12">
+        <v>34.0</v>
+      </c>
       <c r="J7" s="13"/>
       <c r="K7" s="15"/>
       <c r="L7" s="13"/>
@@ -1032,12 +1050,12 @@
       <c r="Z7" s="18"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="12">
         <v>31.0</v>
@@ -1055,7 +1073,9 @@
       <c r="H8" s="13">
         <v>38.0</v>
       </c>
-      <c r="I8" s="12"/>
+      <c r="I8" s="12">
+        <v>34.0</v>
+      </c>
       <c r="J8" s="13"/>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
@@ -1075,12 +1095,12 @@
       <c r="Z8" s="16"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>173</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" s="12">
         <v>34.0</v>
@@ -1100,7 +1120,9 @@
       <c r="H9" s="13">
         <v>35.0</v>
       </c>
-      <c r="I9" s="15"/>
+      <c r="I9" s="12">
+        <v>24.0</v>
+      </c>
       <c r="J9" s="14"/>
       <c r="K9" s="15"/>
       <c r="L9" s="13"/>
@@ -1120,12 +1142,12 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>191</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" s="12">
         <v>21.0</v>
@@ -1137,7 +1159,9 @@
       <c r="H10" s="13">
         <v>31.0</v>
       </c>
-      <c r="I10" s="12"/>
+      <c r="I10" s="12">
+        <v>37.0</v>
+      </c>
       <c r="J10" s="13"/>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
@@ -1157,12 +1181,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="12">
         <v>36.0</v>
@@ -1207,7 +1231,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="12">
         <v>35.0</v>
@@ -1225,7 +1249,9 @@
       <c r="H12" s="13">
         <v>36.0</v>
       </c>
-      <c r="I12" s="12"/>
+      <c r="I12" s="12">
+        <v>39.0</v>
+      </c>
       <c r="J12" s="13"/>
       <c r="K12" s="15"/>
       <c r="L12" s="13"/>
@@ -1245,12 +1271,12 @@
       <c r="Z12" s="18"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>165</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C13" s="12">
         <v>34.0</v>
@@ -1264,7 +1290,9 @@
       <c r="H13" s="13">
         <v>30.0</v>
       </c>
-      <c r="I13" s="15"/>
+      <c r="I13" s="12">
+        <v>27.0</v>
+      </c>
       <c r="J13" s="14"/>
       <c r="K13" s="15"/>
       <c r="L13" s="14"/>
@@ -1284,12 +1312,12 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>86</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="12">
         <v>33.0</v>
@@ -1307,7 +1335,9 @@
       <c r="H14" s="13">
         <v>36.0</v>
       </c>
-      <c r="I14" s="12"/>
+      <c r="I14" s="12">
+        <v>30.0</v>
+      </c>
       <c r="J14" s="13"/>
       <c r="K14" s="12"/>
       <c r="L14" s="13"/>
@@ -1327,12 +1357,12 @@
       <c r="Z14" s="18"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>163</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -1365,7 +1395,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
@@ -1381,7 +1411,9 @@
       <c r="H16" s="13">
         <v>34.0</v>
       </c>
-      <c r="I16" s="12"/>
+      <c r="I16" s="12">
+        <v>31.0</v>
+      </c>
       <c r="J16" s="13"/>
       <c r="K16" s="15"/>
       <c r="L16" s="13"/>
@@ -1401,12 +1433,12 @@
       <c r="Z16" s="18"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>128</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C17" s="18">
         <v>26.0</v>
@@ -1420,7 +1452,9 @@
       <c r="H17" s="13">
         <v>32.0</v>
       </c>
-      <c r="I17" s="12"/>
+      <c r="I17" s="12">
+        <v>29.0</v>
+      </c>
       <c r="J17" s="13"/>
       <c r="K17" s="15"/>
       <c r="L17" s="14"/>
@@ -1440,12 +1474,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="12">
         <v>31.0</v>
@@ -1461,7 +1495,9 @@
       <c r="H18" s="12">
         <v>28.0</v>
       </c>
-      <c r="I18" s="12"/>
+      <c r="I18" s="12">
+        <v>35.0</v>
+      </c>
       <c r="J18" s="15"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -1481,7 +1517,7 @@
       <c r="Z18" s="12"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>126</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -1512,27 +1548,29 @@
     </row>
     <row r="20" ht="72.0" customHeight="1">
       <c r="B20" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E20" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="F20" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="I20" s="24"/>
+      <c r="I20" s="24" t="s">
+        <v>34</v>
+      </c>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
@@ -1554,7 +1592,7 @@
     </row>
     <row r="21">
       <c r="B21" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C21" s="27">
         <v>36.0</v>
@@ -1574,7 +1612,9 @@
       <c r="H21" s="27">
         <v>41.0</v>
       </c>
-      <c r="I21" s="27"/>
+      <c r="I21" s="27">
+        <v>40.0</v>
+      </c>
       <c r="J21" s="27"/>
       <c r="K21" s="27"/>
       <c r="L21" s="27"/>
@@ -1616,28 +1656,30 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H3" s="3"/>
+        <v>55</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
@@ -1660,87 +1702,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
@@ -1777,7 +1819,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C6" s="12">
         <v>38.0</v>
@@ -1816,7 +1858,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
@@ -1831,7 +1873,9 @@
       <c r="G7" s="12">
         <v>43.0</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="13">
+        <v>30.0</v>
+      </c>
       <c r="I7" s="12"/>
       <c r="J7" s="14"/>
       <c r="K7" s="12"/>
@@ -1852,12 +1896,12 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>125</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="12">
         <v>28.0</v>
@@ -1872,7 +1916,9 @@
       <c r="G8" s="12">
         <v>36.0</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="13">
+        <v>29.0</v>
+      </c>
       <c r="I8" s="12"/>
       <c r="J8" s="13"/>
       <c r="K8" s="15"/>
@@ -1893,12 +1939,12 @@
       <c r="Z8" s="18"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13">
@@ -1937,7 +1983,7 @@
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
@@ -1946,7 +1992,9 @@
         <v>35.0</v>
       </c>
       <c r="G10" s="12"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="13">
+        <v>32.0</v>
+      </c>
       <c r="I10" s="15"/>
       <c r="J10" s="14"/>
       <c r="K10" s="12"/>
@@ -1967,12 +2015,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C11" s="12">
         <v>33.0</v>
@@ -2013,7 +2061,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -2050,7 +2098,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C13" s="12">
         <v>33.0</v>
@@ -2063,7 +2111,9 @@
       <c r="G13" s="12">
         <v>26.0</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="13">
+        <v>31.0</v>
+      </c>
       <c r="I13" s="15"/>
       <c r="J13" s="13"/>
       <c r="K13" s="12"/>
@@ -2084,12 +2134,12 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>82</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" s="12">
         <v>29.0</v>
@@ -2104,7 +2154,9 @@
       <c r="G14" s="12">
         <v>31.0</v>
       </c>
-      <c r="H14" s="14"/>
+      <c r="H14" s="13">
+        <v>27.0</v>
+      </c>
       <c r="I14" s="15"/>
       <c r="J14" s="13"/>
       <c r="K14" s="12"/>
@@ -2125,12 +2177,12 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>112</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="12">
         <v>28.0</v>
@@ -2147,7 +2199,9 @@
       <c r="G15" s="12">
         <v>34.0</v>
       </c>
-      <c r="H15" s="14"/>
+      <c r="H15" s="13">
+        <v>31.0</v>
+      </c>
       <c r="I15" s="15"/>
       <c r="J15" s="14"/>
       <c r="K15" s="15"/>
@@ -2168,12 +2222,12 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>175</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" s="12">
         <v>24.0</v>
@@ -2188,7 +2242,9 @@
       <c r="G16" s="12">
         <v>35.0</v>
       </c>
-      <c r="H16" s="13"/>
+      <c r="H16" s="13">
+        <v>34.0</v>
+      </c>
       <c r="I16" s="15"/>
       <c r="J16" s="14"/>
       <c r="K16" s="15"/>
@@ -2209,12 +2265,12 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>122</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C17" s="12">
         <v>31.0</v>
@@ -2255,7 +2311,7 @@
     </row>
     <row r="18">
       <c r="B18" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C18" s="12">
         <v>35.0</v>
@@ -2296,7 +2352,7 @@
     </row>
     <row r="19">
       <c r="B19" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C19" s="12">
         <v>33.0</v>
@@ -2311,7 +2367,9 @@
       <c r="G19" s="12">
         <v>37.0</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="13">
+        <v>32.0</v>
+      </c>
       <c r="I19" s="12"/>
       <c r="J19" s="13"/>
       <c r="K19" s="15"/>
@@ -2332,12 +2390,12 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>136</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C20" s="12">
         <v>27.0</v>
@@ -2346,7 +2404,9 @@
       <c r="E20" s="12"/>
       <c r="F20" s="14"/>
       <c r="G20" s="12"/>
-      <c r="H20" s="13"/>
+      <c r="H20" s="13">
+        <v>29.0</v>
+      </c>
       <c r="I20" s="15"/>
       <c r="J20" s="13"/>
       <c r="K20" s="12"/>
@@ -2367,12 +2427,12 @@
       <c r="Z20" s="18"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C21" s="12">
         <v>31.0</v>
@@ -2411,7 +2471,7 @@
     </row>
     <row r="22">
       <c r="B22" s="28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
@@ -2422,7 +2482,9 @@
       <c r="G22" s="12">
         <v>32.0</v>
       </c>
-      <c r="H22" s="13"/>
+      <c r="H22" s="13">
+        <v>37.0</v>
+      </c>
       <c r="I22" s="12"/>
       <c r="J22" s="13"/>
       <c r="K22" s="12"/>
@@ -2443,7 +2505,7 @@
       <c r="Z22" s="18"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -2474,24 +2536,26 @@
     </row>
     <row r="24" ht="84.75" customHeight="1">
       <c r="B24" s="23" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="H24" s="24"/>
+        <v>45</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>67</v>
+      </c>
       <c r="I24" s="24"/>
       <c r="J24" s="24"/>
       <c r="K24" s="24"/>
@@ -2514,7 +2578,7 @@
     </row>
     <row r="25">
       <c r="B25" s="26" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C25" s="27">
         <v>38.0</v>
@@ -2531,7 +2595,9 @@
       <c r="G25" s="27">
         <v>43.0</v>
       </c>
-      <c r="H25" s="27"/>
+      <c r="H25" s="27">
+        <v>38.0</v>
+      </c>
       <c r="I25" s="27"/>
       <c r="J25" s="27"/>
       <c r="K25" s="27"/>
@@ -2574,18 +2640,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -2594,16 +2660,16 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -2612,7 +2678,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -2621,7 +2687,7 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -2630,7 +2696,7 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -2639,16 +2705,16 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
-        <v>14.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -2657,7 +2723,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -2666,25 +2732,22 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
-        <v>19.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="33"/>
-      <c r="C12" s="34">
-        <v>12.0</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -2693,7 +2756,7 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -2702,7 +2765,7 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -2711,7 +2774,7 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -2720,7 +2783,7 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -2729,7 +2792,7 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="34">
@@ -2738,7 +2801,7 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="34">
@@ -2747,7 +2810,7 @@
     </row>
     <row r="20">
       <c r="A20" s="35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="34">
@@ -2756,7 +2819,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="34">
@@ -2765,7 +2828,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="34">
@@ -2774,7 +2837,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="34">
@@ -2783,7 +2846,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B24" s="36"/>
       <c r="C24" s="37">
@@ -2792,11 +2855,11 @@
     </row>
     <row r="25">
       <c r="A25" s="35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="13">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="26">
@@ -6705,13 +6768,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2">
@@ -6719,10 +6782,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3">
@@ -6730,10 +6793,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="43" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4">
@@ -6741,10 +6804,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
@@ -6752,10 +6815,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
@@ -6763,19 +6826,21 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="13">
         <v>6.0</v>
       </c>
-      <c r="B7" s="43"/>
+      <c r="B7" s="43" t="s">
+        <v>74</v>
+      </c>
       <c r="C7" s="44" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -6783,7 +6848,9 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="43"/>
-      <c r="C8" s="44"/>
+      <c r="C8" s="44" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="13">
@@ -11782,19 +11849,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D1" s="45" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2">
@@ -11908,11 +11975,11 @@
       </c>
       <c r="B7" s="46" t="str">
         <f>'SUNDAY SINGLES'!H24</f>
-        <v/>
-      </c>
-      <c r="C7" s="46" t="str">
+        <v>GAZ LENTON</v>
+      </c>
+      <c r="C7" s="46">
         <f>'SUNDAY SINGLES'!H25</f>
-        <v/>
+        <v>38</v>
       </c>
       <c r="D7" s="47" t="str">
         <f>'THURSDAY SINGLES'!H20</f>
@@ -11937,11 +12004,11 @@
       </c>
       <c r="D8" s="47" t="str">
         <f>'THURSDAY SINGLES'!I20</f>
-        <v/>
-      </c>
-      <c r="E8" s="46" t="str">
+        <v>DAVE BARNETT</v>
+      </c>
+      <c r="E8" s="46">
         <f>'THURSDAY SINGLES'!I$21</f>
-        <v/>
+        <v>40</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
078 Datatype bug fix
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -1424,9 +1424,7 @@
       <c r="B15" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="12">
-        <v>1.0</v>
-      </c>
+      <c r="C15" s="12"/>
       <c r="D15" s="13"/>
       <c r="E15" s="12"/>
       <c r="F15" s="13"/>
@@ -1452,7 +1450,7 @@
       <c r="Z15" s="18"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
079 Game week 9/9 update
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="86">
   <si>
     <t>WINTER GOLF 25/26 - THURSDAY SINGLES</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>27th Nov 25</t>
+  </si>
+  <si>
+    <t>2nd Dec 25</t>
   </si>
   <si>
     <t>NAME</t>
@@ -198,6 +201,9 @@
   </si>
   <si>
     <t>30th Nov 25</t>
+  </si>
+  <si>
+    <t>7th Dec 25</t>
   </si>
   <si>
     <t>MICK SKINNER</t>
@@ -855,7 +861,9 @@
       <c r="K3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="4"/>
+      <c r="L3" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="M3" s="3"/>
       <c r="N3" s="4"/>
       <c r="O3" s="3"/>
@@ -874,87 +882,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13">
@@ -1001,7 +1009,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C6" s="12">
         <v>28.0</v>
@@ -1048,7 +1056,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C7" s="12">
         <v>31.0</v>
@@ -1093,7 +1101,7 @@
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="12">
         <v>31.0</v>
@@ -1140,7 +1148,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="12">
         <v>34.0</v>
@@ -1191,7 +1199,7 @@
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="12">
         <v>21.0</v>
@@ -1230,7 +1238,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" s="12">
         <v>36.0</v>
@@ -1279,7 +1287,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" s="12">
         <v>35.0</v>
@@ -1328,7 +1336,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C13" s="12">
         <v>34.0</v>
@@ -1373,7 +1381,7 @@
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="12">
         <v>33.0</v>
@@ -1422,7 +1430,7 @@
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -1455,7 +1463,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
@@ -1502,7 +1510,7 @@
     </row>
     <row r="17">
       <c r="B17" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C17" s="18">
         <v>26.0</v>
@@ -1545,7 +1553,7 @@
     </row>
     <row r="18">
       <c r="B18" s="21" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="12">
         <v>31.0</v>
@@ -1616,34 +1624,34 @@
     </row>
     <row r="20" ht="72.0" customHeight="1">
       <c r="B20" s="23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="F20" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>38</v>
-      </c>
       <c r="I20" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
@@ -1664,7 +1672,7 @@
     </row>
     <row r="21">
       <c r="B21" s="26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C21" s="27">
         <v>36.0</v>
@@ -1732,37 +1740,39 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="3"/>
+        <v>61</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="3"/>
       <c r="N3" s="4"/>
@@ -1782,87 +1792,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
@@ -1899,7 +1909,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C6" s="12">
         <v>38.0</v>
@@ -1940,7 +1950,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
@@ -1962,7 +1972,9 @@
       <c r="J7" s="13">
         <v>29.0</v>
       </c>
-      <c r="K7" s="12"/>
+      <c r="K7" s="12">
+        <v>24.0</v>
+      </c>
       <c r="L7" s="13"/>
       <c r="M7" s="12"/>
       <c r="N7" s="13"/>
@@ -1980,12 +1992,12 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>184</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C8" s="12">
         <v>28.0</v>
@@ -2028,7 +2040,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13">
@@ -2044,7 +2056,9 @@
       <c r="H9" s="13"/>
       <c r="I9" s="15"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="15"/>
+      <c r="K9" s="12">
+        <v>31.0</v>
+      </c>
       <c r="L9" s="14"/>
       <c r="M9" s="12"/>
       <c r="N9" s="13"/>
@@ -2062,12 +2076,12 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
@@ -2108,7 +2122,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C11" s="12">
         <v>33.0</v>
@@ -2149,7 +2163,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -2188,7 +2202,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C13" s="12">
         <v>33.0</v>
@@ -2231,7 +2245,7 @@
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C14" s="12">
         <v>29.0</v>
@@ -2253,7 +2267,9 @@
       <c r="J14" s="13">
         <v>29.0</v>
       </c>
-      <c r="K14" s="12"/>
+      <c r="K14" s="12">
+        <v>32.0</v>
+      </c>
       <c r="L14" s="14"/>
       <c r="M14" s="12"/>
       <c r="N14" s="13"/>
@@ -2271,12 +2287,12 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>168</v>
+        <v>200</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" s="12">
         <v>28.0</v>
@@ -2323,7 +2339,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="12">
         <v>24.0</v>
@@ -2368,7 +2384,7 @@
     </row>
     <row r="17">
       <c r="B17" s="17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C17" s="12">
         <v>31.0</v>
@@ -2390,7 +2406,9 @@
       <c r="J17" s="13">
         <v>31.0</v>
       </c>
-      <c r="K17" s="12"/>
+      <c r="K17" s="12">
+        <v>30.0</v>
+      </c>
       <c r="L17" s="13"/>
       <c r="M17" s="12"/>
       <c r="N17" s="13"/>
@@ -2408,12 +2426,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>191</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C18" s="12">
         <v>35.0</v>
@@ -2456,7 +2474,7 @@
     </row>
     <row r="19">
       <c r="B19" s="17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C19" s="12">
         <v>33.0</v>
@@ -2480,7 +2498,9 @@
       <c r="J19" s="13">
         <v>28.0</v>
       </c>
-      <c r="K19" s="15"/>
+      <c r="K19" s="12">
+        <v>32.0</v>
+      </c>
       <c r="L19" s="13"/>
       <c r="M19" s="15"/>
       <c r="N19" s="14"/>
@@ -2498,12 +2518,12 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>228</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C20" s="12">
         <v>27.0</v>
@@ -2521,7 +2541,9 @@
       <c r="J20" s="13">
         <v>29.0</v>
       </c>
-      <c r="K20" s="12"/>
+      <c r="K20" s="12">
+        <v>28.0</v>
+      </c>
       <c r="L20" s="14"/>
       <c r="M20" s="12"/>
       <c r="N20" s="13"/>
@@ -2539,12 +2561,12 @@
       <c r="Z20" s="18"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>116</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C21" s="12">
         <v>31.0</v>
@@ -2562,7 +2584,9 @@
         <v>29.0</v>
       </c>
       <c r="J21" s="13"/>
-      <c r="K21" s="15"/>
+      <c r="K21" s="12">
+        <v>27.0</v>
+      </c>
       <c r="L21" s="14"/>
       <c r="M21" s="15"/>
       <c r="N21" s="13"/>
@@ -2580,12 +2604,12 @@
       <c r="Z21" s="18"/>
       <c r="AA21" s="14">
         <f t="shared" si="1"/>
-        <v>118</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
@@ -2652,33 +2676,35 @@
     </row>
     <row r="24" ht="84.75" customHeight="1">
       <c r="B24" s="23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="K24" s="24"/>
+        <v>74</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>70</v>
+      </c>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
       <c r="N24" s="24"/>
@@ -2698,7 +2724,7 @@
     </row>
     <row r="25">
       <c r="B25" s="26" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C25" s="27">
         <v>38.0</v>
@@ -2724,7 +2750,9 @@
       <c r="J25" s="27">
         <v>35.0</v>
       </c>
-      <c r="K25" s="27"/>
+      <c r="K25" s="27">
+        <v>32.0</v>
+      </c>
       <c r="L25" s="27"/>
       <c r="M25" s="27"/>
       <c r="N25" s="27"/>
@@ -2764,18 +2792,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -2784,7 +2812,7 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -2793,7 +2821,7 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -2802,7 +2830,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -2811,7 +2839,7 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -2820,7 +2848,7 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -2829,7 +2857,7 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -2838,7 +2866,7 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -2847,7 +2875,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -2856,7 +2884,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -2865,7 +2893,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="35">
@@ -2874,7 +2902,7 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -2883,7 +2911,7 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -2892,7 +2920,7 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -2901,7 +2929,7 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -2910,7 +2938,7 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -2919,7 +2947,7 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="34">
@@ -2928,25 +2956,25 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="34">
-        <v>-2.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="34">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="34">
@@ -2955,7 +2983,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="34">
@@ -2964,7 +2992,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="34">
@@ -2973,7 +3001,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="38">
@@ -2982,7 +3010,7 @@
     </row>
     <row r="25">
       <c r="A25" s="36" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="13">
@@ -6895,13 +6923,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2">
@@ -6909,10 +6937,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
@@ -6920,10 +6948,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4">
@@ -6931,10 +6959,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
@@ -6942,10 +6970,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6">
@@ -6953,10 +6981,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7">
@@ -6964,10 +6992,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
@@ -6975,10 +7003,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9">
@@ -6986,19 +7014,21 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="13">
         <v>9.0</v>
       </c>
-      <c r="B10" s="44"/>
+      <c r="B10" s="44" t="s">
+        <v>80</v>
+      </c>
       <c r="C10" s="45" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7007,7 +7037,9 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
+      <c r="C11" s="45" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="13">
@@ -11984,19 +12016,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2">
@@ -12173,11 +12205,11 @@
       </c>
       <c r="B10" s="47" t="str">
         <f>'SUNDAY SINGLES'!K24</f>
-        <v/>
-      </c>
-      <c r="C10" s="47" t="str">
+        <v>CHRIS HARVEY</v>
+      </c>
+      <c r="C10" s="47">
         <f>'SUNDAY SINGLES'!K25</f>
-        <v/>
+        <v>32</v>
       </c>
       <c r="D10" s="48" t="str">
         <f>'THURSDAY SINGLES'!K20</f>

</xml_diff>

<commit_message>
080 Week 10/11 data update
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="88">
   <si>
     <t>WINTER GOLF 25/26 - THURSDAY SINGLES</t>
   </si>
@@ -47,7 +47,10 @@
     <t>27th Nov 25</t>
   </si>
   <si>
-    <t>2nd Dec 25</t>
+    <t>4th Dec 25</t>
+  </si>
+  <si>
+    <t>11th Dec 25</t>
   </si>
   <si>
     <t>NAME</t>
@@ -173,6 +176,9 @@
     <t>WEEKLY WINNER</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>WINNERS SCORE</t>
   </si>
   <si>
@@ -204,6 +210,9 @@
   </si>
   <si>
     <t>7th Dec 25</t>
+  </si>
+  <si>
+    <t>14th Dec 25</t>
   </si>
   <si>
     <t>MICK SKINNER</t>
@@ -242,6 +251,9 @@
     <t>STUART BRYAN</t>
   </si>
   <si>
+    <t>PAUL HANCOX</t>
+  </si>
+  <si>
     <t>WHITE TEES</t>
   </si>
   <si>
@@ -255,12 +267,6 @@
   </si>
   <si>
     <t>THURSDAY NEAREST PIN</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>PAUL HANCOX</t>
   </si>
   <si>
     <t>SUNDAY</t>
@@ -864,7 +870,9 @@
       <c r="L3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="N3" s="4"/>
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
@@ -882,87 +890,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13">
@@ -988,7 +996,9 @@
         <v>29.0</v>
       </c>
       <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
+      <c r="M5" s="12">
+        <v>29.0</v>
+      </c>
       <c r="N5" s="14"/>
       <c r="O5" s="12"/>
       <c r="P5" s="13"/>
@@ -1004,12 +1014,12 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>215</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="12">
         <v>28.0</v>
@@ -1035,7 +1045,9 @@
         <v>29.0</v>
       </c>
       <c r="L6" s="13"/>
-      <c r="M6" s="12"/>
+      <c r="M6" s="12">
+        <v>35.0</v>
+      </c>
       <c r="N6" s="13"/>
       <c r="O6" s="15"/>
       <c r="P6" s="14"/>
@@ -1051,12 +1063,12 @@
       <c r="Z6" s="18"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>191</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="12">
         <v>31.0</v>
@@ -1101,7 +1113,7 @@
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="12">
         <v>31.0</v>
@@ -1148,7 +1160,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="12">
         <v>34.0</v>
@@ -1178,7 +1190,9 @@
         <v>34.0</v>
       </c>
       <c r="L9" s="13"/>
-      <c r="M9" s="12"/>
+      <c r="M9" s="12">
+        <v>24.0</v>
+      </c>
       <c r="N9" s="13"/>
       <c r="O9" s="12"/>
       <c r="P9" s="13"/>
@@ -1194,12 +1208,12 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>274</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="12">
         <v>21.0</v>
@@ -1238,7 +1252,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C11" s="12">
         <v>36.0</v>
@@ -1287,7 +1301,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C12" s="12">
         <v>35.0</v>
@@ -1315,7 +1329,9 @@
         <v>32.0</v>
       </c>
       <c r="L12" s="13"/>
-      <c r="M12" s="12"/>
+      <c r="M12" s="12">
+        <v>32.0</v>
+      </c>
       <c r="N12" s="14"/>
       <c r="O12" s="12"/>
       <c r="P12" s="13"/>
@@ -1331,12 +1347,12 @@
       <c r="Z12" s="18"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>273</v>
+        <v>305</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C13" s="12">
         <v>34.0</v>
@@ -1381,7 +1397,7 @@
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="12">
         <v>33.0</v>
@@ -1409,7 +1425,9 @@
         <v>38.0</v>
       </c>
       <c r="L14" s="13"/>
-      <c r="M14" s="12"/>
+      <c r="M14" s="12">
+        <v>27.0</v>
+      </c>
       <c r="N14" s="13"/>
       <c r="O14" s="12"/>
       <c r="P14" s="13"/>
@@ -1425,12 +1443,12 @@
       <c r="Z14" s="18"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>258</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -1463,7 +1481,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
@@ -1489,7 +1507,9 @@
         <v>34.0</v>
       </c>
       <c r="L16" s="13"/>
-      <c r="M16" s="15"/>
+      <c r="M16" s="12">
+        <v>28.0</v>
+      </c>
       <c r="N16" s="14"/>
       <c r="O16" s="12"/>
       <c r="P16" s="13"/>
@@ -1505,12 +1525,12 @@
       <c r="Z16" s="18"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>214</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C17" s="18">
         <v>26.0</v>
@@ -1553,7 +1573,7 @@
     </row>
     <row r="18">
       <c r="B18" s="21" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="12">
         <v>31.0</v>
@@ -1577,7 +1597,9 @@
         <v>31.0</v>
       </c>
       <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
+      <c r="M18" s="12">
+        <v>36.0</v>
+      </c>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="15"/>
@@ -1593,7 +1615,7 @@
       <c r="Z18" s="12"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>192</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -1624,37 +1646,41 @@
     </row>
     <row r="20" ht="72.0" customHeight="1">
       <c r="B20" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="M20" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="L20" s="24"/>
-      <c r="M20" s="24"/>
       <c r="N20" s="24"/>
       <c r="O20" s="24"/>
       <c r="P20" s="24"/>
@@ -1672,7 +1698,7 @@
     </row>
     <row r="21">
       <c r="B21" s="26" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C21" s="27">
         <v>36.0</v>
@@ -1702,7 +1728,9 @@
         <v>38.0</v>
       </c>
       <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
+      <c r="M21" s="27">
+        <v>36.0</v>
+      </c>
       <c r="N21" s="27"/>
       <c r="O21" s="27"/>
       <c r="P21" s="27"/>
@@ -1740,40 +1768,42 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="L3" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="M3" s="3"/>
       <c r="N3" s="4"/>
       <c r="O3" s="3"/>
@@ -1792,87 +1822,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
@@ -1909,7 +1939,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C6" s="12">
         <v>38.0</v>
@@ -1950,7 +1980,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
@@ -1975,7 +2005,9 @@
       <c r="K7" s="12">
         <v>24.0</v>
       </c>
-      <c r="L7" s="13"/>
+      <c r="L7" s="13">
+        <v>27.0</v>
+      </c>
       <c r="M7" s="12"/>
       <c r="N7" s="13"/>
       <c r="O7" s="15"/>
@@ -1992,12 +2024,12 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>208</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="12">
         <v>28.0</v>
@@ -2040,7 +2072,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13">
@@ -2059,7 +2091,9 @@
       <c r="K9" s="12">
         <v>31.0</v>
       </c>
-      <c r="L9" s="14"/>
+      <c r="L9" s="13">
+        <v>36.0</v>
+      </c>
       <c r="M9" s="12"/>
       <c r="N9" s="13"/>
       <c r="O9" s="12"/>
@@ -2076,12 +2110,12 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>131</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
@@ -2100,7 +2134,9 @@
         <v>33.0</v>
       </c>
       <c r="K10" s="12"/>
-      <c r="L10" s="14"/>
+      <c r="L10" s="13">
+        <v>35.0</v>
+      </c>
       <c r="M10" s="12"/>
       <c r="N10" s="13"/>
       <c r="O10" s="12"/>
@@ -2117,12 +2153,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>132</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C11" s="12">
         <v>33.0</v>
@@ -2163,7 +2199,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -2180,7 +2216,9 @@
         <v>35.0</v>
       </c>
       <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
+      <c r="L12" s="13">
+        <v>37.0</v>
+      </c>
       <c r="M12" s="12"/>
       <c r="N12" s="13"/>
       <c r="O12" s="15"/>
@@ -2197,12 +2235,12 @@
       <c r="Z12" s="18"/>
       <c r="AA12" s="14">
         <f t="shared" si="1"/>
-        <v>98</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C13" s="12">
         <v>33.0</v>
@@ -2223,7 +2261,9 @@
         <v>33.0</v>
       </c>
       <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
+      <c r="L13" s="13">
+        <v>33.0</v>
+      </c>
       <c r="M13" s="15"/>
       <c r="N13" s="13"/>
       <c r="O13" s="12"/>
@@ -2240,12 +2280,12 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>146</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" s="12">
         <v>29.0</v>
@@ -2270,7 +2310,9 @@
       <c r="K14" s="12">
         <v>32.0</v>
       </c>
-      <c r="L14" s="14"/>
+      <c r="L14" s="13">
+        <v>28.0</v>
+      </c>
       <c r="M14" s="12"/>
       <c r="N14" s="13"/>
       <c r="O14" s="12"/>
@@ -2287,12 +2329,12 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="12">
         <v>28.0</v>
@@ -2317,7 +2359,9 @@
       </c>
       <c r="J15" s="14"/>
       <c r="K15" s="15"/>
-      <c r="L15" s="14"/>
+      <c r="L15" s="13">
+        <v>31.0</v>
+      </c>
       <c r="M15" s="15"/>
       <c r="N15" s="14"/>
       <c r="O15" s="15"/>
@@ -2334,12 +2378,12 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>202</v>
+        <v>233</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="12">
         <v>24.0</v>
@@ -2384,7 +2428,7 @@
     </row>
     <row r="17">
       <c r="B17" s="17" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C17" s="12">
         <v>31.0</v>
@@ -2409,7 +2453,9 @@
       <c r="K17" s="12">
         <v>30.0</v>
       </c>
-      <c r="L17" s="13"/>
+      <c r="L17" s="13">
+        <v>29.0</v>
+      </c>
       <c r="M17" s="12"/>
       <c r="N17" s="13"/>
       <c r="O17" s="12"/>
@@ -2426,12 +2472,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>221</v>
+        <v>250</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="17" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C18" s="12">
         <v>35.0</v>
@@ -2474,7 +2520,7 @@
     </row>
     <row r="19">
       <c r="B19" s="17" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C19" s="12">
         <v>33.0</v>
@@ -2501,7 +2547,9 @@
       <c r="K19" s="12">
         <v>32.0</v>
       </c>
-      <c r="L19" s="13"/>
+      <c r="L19" s="13">
+        <v>35.0</v>
+      </c>
       <c r="M19" s="15"/>
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
@@ -2518,12 +2566,12 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>260</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="17" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C20" s="12">
         <v>27.0</v>
@@ -2544,7 +2592,9 @@
       <c r="K20" s="12">
         <v>28.0</v>
       </c>
-      <c r="L20" s="14"/>
+      <c r="L20" s="13">
+        <v>30.0</v>
+      </c>
       <c r="M20" s="12"/>
       <c r="N20" s="13"/>
       <c r="O20" s="12"/>
@@ -2561,12 +2611,12 @@
       <c r="Z20" s="18"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>144</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C21" s="12">
         <v>31.0</v>
@@ -2587,7 +2637,9 @@
       <c r="K21" s="12">
         <v>27.0</v>
       </c>
-      <c r="L21" s="14"/>
+      <c r="L21" s="13">
+        <v>15.0</v>
+      </c>
       <c r="M21" s="15"/>
       <c r="N21" s="13"/>
       <c r="O21" s="15"/>
@@ -2604,12 +2656,12 @@
       <c r="Z21" s="18"/>
       <c r="AA21" s="14">
         <f t="shared" si="1"/>
-        <v>145</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
@@ -2628,7 +2680,9 @@
         <v>33.0</v>
       </c>
       <c r="K22" s="12"/>
-      <c r="L22" s="14"/>
+      <c r="L22" s="13">
+        <v>30.0</v>
+      </c>
       <c r="M22" s="12"/>
       <c r="N22" s="13"/>
       <c r="O22" s="12"/>
@@ -2645,7 +2699,7 @@
       <c r="Z22" s="18"/>
       <c r="AA22" s="14">
         <f t="shared" si="1"/>
-        <v>135</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" ht="9.0" customHeight="1">
@@ -2676,36 +2730,38 @@
     </row>
     <row r="24" ht="84.75" customHeight="1">
       <c r="B24" s="23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H24" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="J24" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="K24" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I24" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="K24" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="L24" s="24"/>
+      <c r="L24" s="24" t="s">
+        <v>78</v>
+      </c>
       <c r="M24" s="24"/>
       <c r="N24" s="24"/>
       <c r="O24" s="24"/>
@@ -2724,7 +2780,7 @@
     </row>
     <row r="25">
       <c r="B25" s="26" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C25" s="27">
         <v>38.0</v>
@@ -2753,7 +2809,9 @@
       <c r="K25" s="27">
         <v>32.0</v>
       </c>
-      <c r="L25" s="27"/>
+      <c r="L25" s="27">
+        <v>38.0</v>
+      </c>
       <c r="M25" s="27"/>
       <c r="N25" s="27"/>
       <c r="O25" s="27"/>
@@ -2792,27 +2850,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
-        <v>15.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -2821,7 +2879,7 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -2830,7 +2888,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -2839,7 +2897,7 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -2848,7 +2906,7 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -2857,7 +2915,7 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -2866,7 +2924,7 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -2875,7 +2933,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -2884,7 +2942,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -2893,7 +2951,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="35">
@@ -2902,7 +2960,7 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -2911,7 +2969,7 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -2920,7 +2978,7 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -2929,7 +2987,7 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -2938,7 +2996,7 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -2947,7 +3005,7 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="34">
@@ -2956,7 +3014,7 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="34">
@@ -2965,7 +3023,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="34">
@@ -2974,7 +3032,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="34">
@@ -2983,7 +3041,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="34">
@@ -2992,7 +3050,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="34">
@@ -3001,7 +3059,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="38">
@@ -3010,7 +3068,7 @@
     </row>
     <row r="25">
       <c r="A25" s="36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="13">
@@ -6923,13 +6981,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2">
@@ -6937,10 +6995,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
@@ -6948,10 +7006,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4">
@@ -6959,10 +7017,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
@@ -6970,10 +7028,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6">
@@ -6981,10 +7039,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7">
@@ -6992,10 +7050,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8">
@@ -7003,10 +7061,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9">
@@ -7014,10 +7072,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
@@ -7025,10 +7083,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7036,9 +7094,11 @@
       <c r="A11" s="13">
         <v>10.0</v>
       </c>
-      <c r="B11" s="44"/>
+      <c r="B11" s="44" t="s">
+        <v>67</v>
+      </c>
       <c r="C11" s="45" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12">
@@ -7046,7 +7106,9 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="44"/>
-      <c r="C12" s="45"/>
+      <c r="C12" s="45" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="13">
@@ -12016,19 +12078,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
@@ -12226,15 +12288,15 @@
       </c>
       <c r="B11" s="47" t="str">
         <f>'SUNDAY SINGLES'!L24</f>
-        <v/>
-      </c>
-      <c r="C11" s="47" t="str">
+        <v>PAUL HANCOX</v>
+      </c>
+      <c r="C11" s="47">
         <f>'SUNDAY SINGLES'!L25</f>
-        <v/>
+        <v>38</v>
       </c>
       <c r="D11" s="48" t="str">
         <f>'THURSDAY SINGLES'!L20</f>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="E11" s="47" t="str">
         <f>'THURSDAY SINGLES'!L$21</f>
@@ -12255,11 +12317,11 @@
       </c>
       <c r="D12" s="48" t="str">
         <f>'THURSDAY SINGLES'!M20</f>
-        <v/>
-      </c>
-      <c r="E12" s="47" t="str">
+        <v>TONY SLATER</v>
+      </c>
+      <c r="E12" s="47">
         <f>'THURSDAY SINGLES'!M21</f>
-        <v/>
+        <v>36</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
081 Week 11/11 update
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="90">
   <si>
     <t>WINTER GOLF 25/26 - THURSDAY SINGLES</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>11th Dec 25</t>
+  </si>
+  <si>
+    <t>18th Dec 25</t>
   </si>
   <si>
     <t>NAME</t>
@@ -213,6 +216,9 @@
   </si>
   <si>
     <t>14th Dec 25</t>
+  </si>
+  <si>
+    <t>21st Dec 25</t>
   </si>
   <si>
     <t>MICK SKINNER</t>
@@ -873,7 +879,9 @@
       <c r="M3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="4"/>
+      <c r="N3" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="3"/>
@@ -890,87 +898,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13">
@@ -1019,7 +1027,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="12">
         <v>28.0</v>
@@ -1068,7 +1076,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C7" s="12">
         <v>31.0</v>
@@ -1113,7 +1121,7 @@
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="12">
         <v>31.0</v>
@@ -1160,7 +1168,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" s="12">
         <v>34.0</v>
@@ -1213,7 +1221,7 @@
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="12">
         <v>21.0</v>
@@ -1252,7 +1260,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11" s="12">
         <v>36.0</v>
@@ -1301,7 +1309,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" s="12">
         <v>35.0</v>
@@ -1352,7 +1360,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" s="12">
         <v>34.0</v>
@@ -1397,7 +1405,7 @@
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C14" s="12">
         <v>33.0</v>
@@ -1448,7 +1456,7 @@
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -1481,7 +1489,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
@@ -1530,7 +1538,7 @@
     </row>
     <row r="17">
       <c r="B17" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C17" s="18">
         <v>26.0</v>
@@ -1573,7 +1581,7 @@
     </row>
     <row r="18">
       <c r="B18" s="21" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C18" s="12">
         <v>31.0</v>
@@ -1646,42 +1654,44 @@
     </row>
     <row r="20" ht="72.0" customHeight="1">
       <c r="B20" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="M20" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>38</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="M20" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="N20" s="24"/>
+      <c r="N20" s="24" t="s">
+        <v>54</v>
+      </c>
       <c r="O20" s="24"/>
       <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
@@ -1698,7 +1708,7 @@
     </row>
     <row r="21">
       <c r="B21" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C21" s="27">
         <v>36.0</v>
@@ -1768,43 +1778,45 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="M3" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="N3" s="4"/>
       <c r="O3" s="3"/>
       <c r="P3" s="4"/>
@@ -1822,87 +1834,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
@@ -1939,7 +1951,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C6" s="12">
         <v>38.0</v>
@@ -1959,7 +1971,9 @@
       <c r="J6" s="13"/>
       <c r="K6" s="12"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="12"/>
+      <c r="M6" s="12">
+        <v>39.0</v>
+      </c>
       <c r="N6" s="13"/>
       <c r="O6" s="12"/>
       <c r="P6" s="14"/>
@@ -1975,12 +1989,12 @@
       <c r="Z6" s="16"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>149</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
@@ -2008,7 +2022,9 @@
       <c r="L7" s="13">
         <v>27.0</v>
       </c>
-      <c r="M7" s="12"/>
+      <c r="M7" s="12">
+        <v>21.0</v>
+      </c>
       <c r="N7" s="13"/>
       <c r="O7" s="15"/>
       <c r="P7" s="13"/>
@@ -2024,12 +2040,12 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>235</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="12">
         <v>28.0</v>
@@ -2072,7 +2088,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13">
@@ -2115,7 +2131,7 @@
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
@@ -2158,7 +2174,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C11" s="12">
         <v>33.0</v>
@@ -2199,7 +2215,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -2240,7 +2256,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C13" s="12">
         <v>33.0</v>
@@ -2264,7 +2280,9 @@
       <c r="L13" s="13">
         <v>33.0</v>
       </c>
-      <c r="M13" s="15"/>
+      <c r="M13" s="12">
+        <v>31.0</v>
+      </c>
       <c r="N13" s="13"/>
       <c r="O13" s="12"/>
       <c r="P13" s="14"/>
@@ -2280,12 +2298,12 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>179</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="12">
         <v>29.0</v>
@@ -2313,7 +2331,9 @@
       <c r="L14" s="13">
         <v>28.0</v>
       </c>
-      <c r="M14" s="12"/>
+      <c r="M14" s="12">
+        <v>35.0</v>
+      </c>
       <c r="N14" s="13"/>
       <c r="O14" s="12"/>
       <c r="P14" s="13"/>
@@ -2329,12 +2349,12 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>228</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="12">
         <v>28.0</v>
@@ -2383,7 +2403,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C16" s="12">
         <v>24.0</v>
@@ -2428,7 +2448,7 @@
     </row>
     <row r="17">
       <c r="B17" s="17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C17" s="12">
         <v>31.0</v>
@@ -2477,7 +2497,7 @@
     </row>
     <row r="18">
       <c r="B18" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C18" s="12">
         <v>35.0</v>
@@ -2520,7 +2540,7 @@
     </row>
     <row r="19">
       <c r="B19" s="17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C19" s="12">
         <v>33.0</v>
@@ -2550,7 +2570,9 @@
       <c r="L19" s="13">
         <v>35.0</v>
       </c>
-      <c r="M19" s="15"/>
+      <c r="M19" s="12">
+        <v>31.0</v>
+      </c>
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
       <c r="P19" s="14"/>
@@ -2566,12 +2588,12 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>295</v>
+        <v>326</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C20" s="12">
         <v>27.0</v>
@@ -2595,7 +2617,9 @@
       <c r="L20" s="13">
         <v>30.0</v>
       </c>
-      <c r="M20" s="12"/>
+      <c r="M20" s="12">
+        <v>28.0</v>
+      </c>
       <c r="N20" s="13"/>
       <c r="O20" s="12"/>
       <c r="P20" s="14"/>
@@ -2611,12 +2635,12 @@
       <c r="Z20" s="18"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>174</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C21" s="12">
         <v>31.0</v>
@@ -2661,7 +2685,7 @@
     </row>
     <row r="22">
       <c r="B22" s="28" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
@@ -2730,39 +2754,41 @@
     </row>
     <row r="24" ht="84.75" customHeight="1">
       <c r="B24" s="23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L24" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="M24" s="24"/>
+        <v>80</v>
+      </c>
+      <c r="M24" s="24" t="s">
+        <v>68</v>
+      </c>
       <c r="N24" s="24"/>
       <c r="O24" s="24"/>
       <c r="P24" s="24"/>
@@ -2780,7 +2806,7 @@
     </row>
     <row r="25">
       <c r="B25" s="26" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" s="27">
         <v>38.0</v>
@@ -2812,7 +2838,9 @@
       <c r="L25" s="27">
         <v>38.0</v>
       </c>
-      <c r="M25" s="27"/>
+      <c r="M25" s="27">
+        <v>39.0</v>
+      </c>
       <c r="N25" s="27"/>
       <c r="O25" s="27"/>
       <c r="P25" s="27"/>
@@ -2850,18 +2878,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -2870,7 +2898,7 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -2879,7 +2907,7 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -2888,7 +2916,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -2897,7 +2925,7 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -2906,7 +2934,7 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -2915,7 +2943,7 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -2924,7 +2952,7 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -2933,7 +2961,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -2942,7 +2970,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -2951,7 +2979,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="35">
@@ -2960,7 +2988,7 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -2969,7 +2997,7 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -2978,7 +3006,7 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -2987,7 +3015,7 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -2996,7 +3024,7 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -3005,7 +3033,7 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="34">
@@ -3014,7 +3042,7 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="34">
@@ -3023,7 +3051,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="34">
@@ -3032,7 +3060,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="34">
@@ -3041,7 +3069,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="34">
@@ -3050,7 +3078,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="34">
@@ -3059,7 +3087,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="38">
@@ -3068,7 +3096,7 @@
     </row>
     <row r="25">
       <c r="A25" s="36" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="13">
@@ -6981,13 +7009,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2">
@@ -6995,10 +7023,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
@@ -7006,10 +7034,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
@@ -7017,10 +7045,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5">
@@ -7028,10 +7056,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6">
@@ -7039,10 +7067,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
@@ -7050,10 +7078,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8">
@@ -7061,10 +7089,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9">
@@ -7072,10 +7100,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
@@ -7083,10 +7111,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7095,19 +7123,21 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="13">
         <v>11.0</v>
       </c>
-      <c r="B12" s="44"/>
+      <c r="B12" s="44" t="s">
+        <v>54</v>
+      </c>
       <c r="C12" s="45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13">
@@ -7115,7 +7145,9 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="44"/>
-      <c r="C13" s="45"/>
+      <c r="C13" s="45" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="13">
@@ -12078,19 +12110,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2">
@@ -12309,11 +12341,11 @@
       </c>
       <c r="B12" s="47" t="str">
         <f>'SUNDAY SINGLES'!M24</f>
-        <v/>
-      </c>
-      <c r="C12" s="47" t="str">
+        <v>MICK SKINNER</v>
+      </c>
+      <c r="C12" s="47">
         <f>'SUNDAY SINGLES'!M25</f>
-        <v/>
+        <v>39</v>
       </c>
       <c r="D12" s="48" t="str">
         <f>'THURSDAY SINGLES'!M20</f>
@@ -12338,7 +12370,7 @@
       </c>
       <c r="D13" s="48" t="str">
         <f>'THURSDAY SINGLES'!N20</f>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="E13" s="47" t="str">
         <f>'THURSDAY SINGLES'!N$21</f>

</xml_diff>

<commit_message>
082 Week 11/14 data update
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="THURSDAY SINGLES" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="SUNDAY SINGLES" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="HANDICAPS" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="NEAREST PIN" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="xxxDO NOT EDITxxx" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="THURSDAY SINGLES" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="SUNDAY SINGLES" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="HANDICAPS" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="NEAREST PIN" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="xxxDO NOT EDITxxx" sheetId="5" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
   <si>
     <t>WINTER GOLF 25/26 - THURSDAY SINGLES</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>18th Dec 25</t>
+  </si>
+  <si>
+    <t>8th Jan 26</t>
+  </si>
+  <si>
+    <t>15th Jan 26</t>
   </si>
   <si>
     <t>NAME</t>
@@ -219,6 +225,15 @@
   </si>
   <si>
     <t>21st Dec 25</t>
+  </si>
+  <si>
+    <t>4th Jan 26</t>
+  </si>
+  <si>
+    <t>11th Jan 26</t>
+  </si>
+  <si>
+    <t>18th Jan 26</t>
   </si>
   <si>
     <t>MICK SKINNER</t>
@@ -628,6 +643,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
@@ -882,8 +901,12 @@
       <c r="N3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="3"/>
-      <c r="P3" s="4"/>
+      <c r="O3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="4"/>
       <c r="S3" s="3"/>
@@ -898,87 +921,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13">
@@ -1008,8 +1031,12 @@
         <v>29.0</v>
       </c>
       <c r="N5" s="14"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="13"/>
+      <c r="O5" s="12">
+        <v>26.0</v>
+      </c>
+      <c r="P5" s="13">
+        <v>29.0</v>
+      </c>
       <c r="Q5" s="15"/>
       <c r="R5" s="13"/>
       <c r="S5" s="12"/>
@@ -1022,12 +1049,12 @@
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
         <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
-        <v>244</v>
+        <v>299</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" s="12">
         <v>28.0</v>
@@ -1058,7 +1085,9 @@
       </c>
       <c r="N6" s="13"/>
       <c r="O6" s="15"/>
-      <c r="P6" s="14"/>
+      <c r="P6" s="13">
+        <v>32.0</v>
+      </c>
       <c r="Q6" s="12"/>
       <c r="R6" s="13"/>
       <c r="S6" s="12"/>
@@ -1071,12 +1100,12 @@
       <c r="Z6" s="18"/>
       <c r="AA6" s="14">
         <f t="shared" si="1"/>
-        <v>226</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7" s="12">
         <v>31.0</v>
@@ -1103,7 +1132,9 @@
       <c r="M7" s="12"/>
       <c r="N7" s="13"/>
       <c r="O7" s="12"/>
-      <c r="P7" s="14"/>
+      <c r="P7" s="13">
+        <v>33.0</v>
+      </c>
       <c r="Q7" s="15"/>
       <c r="R7" s="13"/>
       <c r="S7" s="12"/>
@@ -1116,12 +1147,12 @@
       <c r="Z7" s="18"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>206</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C8" s="12">
         <v>31.0</v>
@@ -1168,7 +1199,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C9" s="12">
         <v>34.0</v>
@@ -1221,7 +1252,7 @@
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C10" s="12">
         <v>21.0</v>
@@ -1242,7 +1273,9 @@
       <c r="M10" s="12"/>
       <c r="N10" s="13"/>
       <c r="O10" s="15"/>
-      <c r="P10" s="13"/>
+      <c r="P10" s="13">
+        <v>30.0</v>
+      </c>
       <c r="Q10" s="12"/>
       <c r="R10" s="14"/>
       <c r="S10" s="15"/>
@@ -1255,12 +1288,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C11" s="12">
         <v>36.0</v>
@@ -1290,7 +1323,9 @@
       <c r="L11" s="13"/>
       <c r="M11" s="15"/>
       <c r="N11" s="14"/>
-      <c r="O11" s="15"/>
+      <c r="O11" s="12">
+        <v>24.0</v>
+      </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="15"/>
       <c r="R11" s="13"/>
@@ -1304,12 +1339,12 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>224</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C12" s="12">
         <v>35.0</v>
@@ -1360,7 +1395,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C13" s="12">
         <v>34.0</v>
@@ -1405,7 +1440,7 @@
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" s="12">
         <v>33.0</v>
@@ -1437,8 +1472,12 @@
         <v>27.0</v>
       </c>
       <c r="N14" s="13"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="13"/>
+      <c r="O14" s="12">
+        <v>25.0</v>
+      </c>
+      <c r="P14" s="13">
+        <v>32.0</v>
+      </c>
       <c r="Q14" s="12"/>
       <c r="R14" s="13"/>
       <c r="S14" s="12"/>
@@ -1451,12 +1490,12 @@
       <c r="Z14" s="18"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>285</v>
+        <v>342</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -1489,7 +1528,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="13"/>
@@ -1519,8 +1558,12 @@
         <v>28.0</v>
       </c>
       <c r="N16" s="14"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="13"/>
+      <c r="O16" s="12">
+        <v>31.0</v>
+      </c>
+      <c r="P16" s="13">
+        <v>29.0</v>
+      </c>
       <c r="Q16" s="15"/>
       <c r="R16" s="14"/>
       <c r="S16" s="12"/>
@@ -1533,12 +1576,12 @@
       <c r="Z16" s="18"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>242</v>
+        <v>302</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="18">
         <v>26.0</v>
@@ -1562,8 +1605,12 @@
       <c r="L17" s="14"/>
       <c r="M17" s="15"/>
       <c r="N17" s="14"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="13"/>
+      <c r="O17" s="12">
+        <v>29.0</v>
+      </c>
+      <c r="P17" s="13">
+        <v>34.0</v>
+      </c>
       <c r="Q17" s="15"/>
       <c r="R17" s="13"/>
       <c r="S17" s="15"/>
@@ -1576,12 +1623,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>150</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C18" s="12">
         <v>31.0</v>
@@ -1610,7 +1657,9 @@
       </c>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
-      <c r="P18" s="15"/>
+      <c r="P18" s="12">
+        <v>29.0</v>
+      </c>
       <c r="Q18" s="12"/>
       <c r="R18" s="15"/>
       <c r="S18" s="15"/>
@@ -1623,7 +1672,7 @@
       <c r="Z18" s="12"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>228</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" ht="9.0" customHeight="1">
@@ -1654,46 +1703,50 @@
     </row>
     <row r="20" ht="72.0" customHeight="1">
       <c r="B20" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="O20" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="P20" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="M20" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="N20" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
       <c r="S20" s="24"/>
@@ -1708,7 +1761,7 @@
     </row>
     <row r="21">
       <c r="B21" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C21" s="27">
         <v>36.0</v>
@@ -1742,8 +1795,12 @@
         <v>36.0</v>
       </c>
       <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
+      <c r="O21" s="27">
+        <v>31.0</v>
+      </c>
+      <c r="P21" s="27">
+        <v>34.0</v>
+      </c>
       <c r="Q21" s="27"/>
       <c r="R21" s="27"/>
       <c r="S21" s="27"/>
@@ -1778,48 +1835,54 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="4"/>
       <c r="S3" s="3"/>
@@ -1834,87 +1897,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
@@ -1951,7 +2014,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C6" s="12">
         <v>38.0</v>
@@ -1994,7 +2057,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
@@ -2045,7 +2108,7 @@
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C8" s="12">
         <v>28.0</v>
@@ -2088,7 +2151,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13">
@@ -2131,7 +2194,7 @@
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
@@ -2174,7 +2237,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C11" s="12">
         <v>33.0</v>
@@ -2215,7 +2278,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -2256,7 +2319,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C13" s="12">
         <v>33.0</v>
@@ -2303,7 +2366,7 @@
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C14" s="12">
         <v>29.0</v>
@@ -2354,7 +2417,7 @@
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15" s="12">
         <v>28.0</v>
@@ -2403,7 +2466,7 @@
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C16" s="12">
         <v>24.0</v>
@@ -2448,7 +2511,7 @@
     </row>
     <row r="17">
       <c r="B17" s="17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C17" s="12">
         <v>31.0</v>
@@ -2497,7 +2560,7 @@
     </row>
     <row r="18">
       <c r="B18" s="17" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C18" s="12">
         <v>35.0</v>
@@ -2540,7 +2603,7 @@
     </row>
     <row r="19">
       <c r="B19" s="17" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C19" s="12">
         <v>33.0</v>
@@ -2593,7 +2656,7 @@
     </row>
     <row r="20">
       <c r="B20" s="17" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C20" s="12">
         <v>27.0</v>
@@ -2640,7 +2703,7 @@
     </row>
     <row r="21">
       <c r="B21" s="17" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C21" s="12">
         <v>31.0</v>
@@ -2685,7 +2748,7 @@
     </row>
     <row r="22">
       <c r="B22" s="28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
@@ -2754,44 +2817,50 @@
     </row>
     <row r="24" ht="84.75" customHeight="1">
       <c r="B24" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D24" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="G24" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="F24" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="I24" s="24" t="s">
-        <v>68</v>
-      </c>
       <c r="J24" s="24" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="L24" s="24" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24"/>
+        <v>73</v>
+      </c>
+      <c r="N24" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="O24" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="P24" s="24" t="s">
+        <v>56</v>
+      </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="24"/>
       <c r="S24" s="24"/>
@@ -2806,7 +2875,7 @@
     </row>
     <row r="25">
       <c r="B25" s="26" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C25" s="27">
         <v>38.0</v>
@@ -2878,27 +2947,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -2907,7 +2976,7 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -2916,7 +2985,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -2925,7 +2994,7 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -2934,7 +3003,7 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -2943,7 +3012,7 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -2952,7 +3021,7 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -2961,7 +3030,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -2970,7 +3039,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -2979,7 +3048,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="35">
@@ -2988,7 +3057,7 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -2997,7 +3066,7 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -3006,25 +3075,25 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
-        <v>19.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -3033,16 +3102,16 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="34">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="34">
@@ -3051,7 +3120,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="34">
@@ -3060,7 +3129,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="34">
@@ -3069,7 +3138,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="34">
@@ -3078,16 +3147,16 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="34">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="38">
@@ -3096,7 +3165,7 @@
     </row>
     <row r="25">
       <c r="A25" s="36" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="13">
@@ -7009,13 +7078,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2">
@@ -7023,10 +7092,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
@@ -7034,10 +7103,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
@@ -7045,10 +7114,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -7056,10 +7125,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
@@ -7067,10 +7136,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
@@ -7078,10 +7147,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8">
@@ -7089,10 +7158,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
@@ -7100,10 +7169,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10">
@@ -7111,10 +7180,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7123,10 +7192,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
@@ -7134,34 +7203,44 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="13">
         <v>12.0</v>
       </c>
-      <c r="B13" s="44"/>
+      <c r="B13" s="44" t="s">
+        <v>56</v>
+      </c>
       <c r="C13" s="45" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="13">
         <v>13.0</v>
       </c>
-      <c r="B14" s="44"/>
-      <c r="C14" s="45"/>
+      <c r="B14" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="13">
         <v>14.0</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="45"/>
+      <c r="B15" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="13">
@@ -12110,19 +12189,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2">
@@ -12362,7 +12441,7 @@
       </c>
       <c r="B13" s="47" t="str">
         <f>'SUNDAY SINGLES'!N24</f>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="C13" s="47" t="str">
         <f>'SUNDAY SINGLES'!N25</f>
@@ -12383,7 +12462,7 @@
       </c>
       <c r="B14" s="47" t="str">
         <f>'SUNDAY SINGLES'!O24</f>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="C14" s="47" t="str">
         <f>'SUNDAY SINGLES'!O25</f>
@@ -12391,11 +12470,11 @@
       </c>
       <c r="D14" s="48" t="str">
         <f>'THURSDAY SINGLES'!O20</f>
-        <v/>
-      </c>
-      <c r="E14" s="47" t="str">
+        <v>LES DOBBINS</v>
+      </c>
+      <c r="E14" s="47">
         <f>'THURSDAY SINGLES'!O21</f>
-        <v/>
+        <v>31</v>
       </c>
     </row>
     <row r="15">
@@ -12404,7 +12483,7 @@
       </c>
       <c r="B15" s="47" t="str">
         <f>'SUNDAY SINGLES'!P24</f>
-        <v/>
+        <v>N/A</v>
       </c>
       <c r="C15" s="47" t="str">
         <f>'SUNDAY SINGLES'!P25</f>
@@ -12412,11 +12491,11 @@
       </c>
       <c r="D15" s="48" t="str">
         <f>'THURSDAY SINGLES'!P20</f>
-        <v/>
-      </c>
-      <c r="E15" s="47" t="str">
+        <v>JODAN HOWARD</v>
+      </c>
+      <c r="E15" s="47">
         <f>'THURSDAY SINGLES'!P21</f>
-        <v/>
+        <v>34</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
083 Week 24,24,24 fix
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="95">
   <si>
     <t>WINTER GOLF 25/26 - THURSDAY SINGLES</t>
   </si>
@@ -170,9 +170,6 @@
     <t>ALBIE GILLESPIE</t>
   </si>
   <si>
-    <t>GORDON PERRIN</t>
-  </si>
-  <si>
     <t>LES DOBBINS</t>
   </si>
   <si>
@@ -279,6 +276,9 @@
   </si>
   <si>
     <t>YELLOW TEES</t>
+  </si>
+  <si>
+    <t>GORDON PERRIN</t>
   </si>
   <si>
     <t>WEEK</t>
@@ -1048,7 +1048,7 @@
       <c r="Y5" s="15"/>
       <c r="Z5" s="16"/>
       <c r="AA5" s="14">
-        <f t="shared" ref="AA5:AA18" si="1">sum(C5:Z5)</f>
+        <f t="shared" ref="AA5:AA17" si="1">sum(C5:Z5)</f>
         <v>299</v>
       </c>
     </row>
@@ -1499,318 +1499,285 @@
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="15"/>
+      <c r="E15" s="12">
+        <v>29.0</v>
+      </c>
+      <c r="F15" s="13">
+        <v>29.0</v>
+      </c>
+      <c r="G15" s="12">
+        <v>36.0</v>
+      </c>
+      <c r="H15" s="13">
+        <v>34.0</v>
+      </c>
+      <c r="I15" s="12">
+        <v>31.0</v>
+      </c>
+      <c r="J15" s="13">
+        <v>21.0</v>
+      </c>
+      <c r="K15" s="12">
+        <v>34.0</v>
+      </c>
       <c r="L15" s="13"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="12"/>
-      <c r="R15" s="13"/>
+      <c r="M15" s="12">
+        <v>28.0</v>
+      </c>
+      <c r="N15" s="14"/>
+      <c r="O15" s="12">
+        <v>31.0</v>
+      </c>
+      <c r="P15" s="13">
+        <v>29.0</v>
+      </c>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="14"/>
       <c r="S15" s="12"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="12"/>
-      <c r="V15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="14"/>
       <c r="W15" s="12"/>
-      <c r="X15" s="14"/>
+      <c r="X15" s="13"/>
       <c r="Y15" s="12"/>
       <c r="Z15" s="18"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="18">
+        <v>26.0</v>
+      </c>
       <c r="D16" s="13"/>
       <c r="E16" s="12">
+        <v>31.0</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="13">
+        <v>32.0</v>
+      </c>
+      <c r="I16" s="12">
         <v>29.0</v>
       </c>
-      <c r="F16" s="13">
-        <v>29.0</v>
-      </c>
-      <c r="G16" s="12">
-        <v>36.0</v>
-      </c>
-      <c r="H16" s="13">
-        <v>34.0</v>
-      </c>
-      <c r="I16" s="12">
-        <v>31.0</v>
-      </c>
-      <c r="J16" s="13">
-        <v>21.0</v>
-      </c>
+      <c r="J16" s="13"/>
       <c r="K16" s="12">
-        <v>34.0</v>
-      </c>
-      <c r="L16" s="13"/>
-      <c r="M16" s="12">
-        <v>28.0</v>
-      </c>
+        <v>32.0</v>
+      </c>
+      <c r="L16" s="14"/>
+      <c r="M16" s="15"/>
       <c r="N16" s="14"/>
       <c r="O16" s="12">
-        <v>31.0</v>
+        <v>29.0</v>
       </c>
       <c r="P16" s="13">
-        <v>29.0</v>
+        <v>34.0</v>
       </c>
       <c r="Q16" s="15"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="12"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="15"/>
       <c r="T16" s="13"/>
-      <c r="U16" s="15"/>
+      <c r="U16" s="12"/>
       <c r="V16" s="14"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="18"/>
+      <c r="W16" s="20"/>
+      <c r="X16" s="14"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>302</v>
+        <v>213</v>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="18">
-        <v>26.0</v>
-      </c>
-      <c r="D17" s="13"/>
+      <c r="C17" s="12">
+        <v>31.0</v>
+      </c>
+      <c r="D17" s="15"/>
       <c r="E17" s="12">
+        <v>32.0</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12">
+        <v>35.0</v>
+      </c>
+      <c r="H17" s="12">
+        <v>28.0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>35.0</v>
+      </c>
+      <c r="J17" s="15"/>
+      <c r="K17" s="12">
         <v>31.0</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="13">
-        <v>32.0</v>
-      </c>
-      <c r="I17" s="12">
+      <c r="L17" s="12"/>
+      <c r="M17" s="12">
+        <v>36.0</v>
+      </c>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12">
         <v>29.0</v>
       </c>
-      <c r="J17" s="13"/>
-      <c r="K17" s="12">
-        <v>32.0</v>
-      </c>
-      <c r="L17" s="14"/>
-      <c r="M17" s="15"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="12">
-        <v>29.0</v>
-      </c>
-      <c r="P17" s="13">
-        <v>34.0</v>
-      </c>
-      <c r="Q17" s="15"/>
-      <c r="R17" s="13"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="15"/>
       <c r="S17" s="15"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="20"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="15"/>
-      <c r="Z17" s="16"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>213</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" s="21" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="18" ht="9.0" customHeight="1">
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="22"/>
+    </row>
+    <row r="19" ht="72.0" customHeight="1">
+      <c r="B19" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C19" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="M19" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="O19" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="P19" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
+      <c r="T19" s="24"/>
+      <c r="U19" s="24"/>
+      <c r="V19" s="24"/>
+      <c r="W19" s="24"/>
+      <c r="X19" s="24"/>
+      <c r="Y19" s="24"/>
+      <c r="Z19" s="24"/>
+      <c r="AA19" s="25"/>
+    </row>
+    <row r="20">
+      <c r="B20" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="27">
+        <v>36.0</v>
+      </c>
+      <c r="D20" s="27">
+        <v>41.0</v>
+      </c>
+      <c r="E20" s="27">
+        <v>38.0</v>
+      </c>
+      <c r="F20" s="27">
+        <v>29.0</v>
+      </c>
+      <c r="G20" s="27">
+        <v>36.0</v>
+      </c>
+      <c r="H20" s="27">
+        <v>41.0</v>
+      </c>
+      <c r="I20" s="27">
+        <v>40.0</v>
+      </c>
+      <c r="J20" s="27">
+        <v>37.0</v>
+      </c>
+      <c r="K20" s="27">
+        <v>38.0</v>
+      </c>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27">
+        <v>36.0</v>
+      </c>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27">
         <v>31.0</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="12">
-        <v>32.0</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12">
-        <v>35.0</v>
-      </c>
-      <c r="H18" s="12">
-        <v>28.0</v>
-      </c>
-      <c r="I18" s="12">
-        <v>35.0</v>
-      </c>
-      <c r="J18" s="15"/>
-      <c r="K18" s="12">
-        <v>31.0</v>
-      </c>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12">
-        <v>36.0</v>
-      </c>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12">
-        <v>29.0</v>
-      </c>
-      <c r="Q18" s="12"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="12"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="12"/>
-      <c r="Y18" s="12"/>
-      <c r="Z18" s="12"/>
-      <c r="AA18" s="14">
-        <f t="shared" si="1"/>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="19" ht="9.0" customHeight="1">
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="22"/>
-      <c r="S19" s="22"/>
-      <c r="T19" s="22"/>
-      <c r="U19" s="22"/>
-      <c r="V19" s="22"/>
-      <c r="W19" s="22"/>
-      <c r="X19" s="22"/>
-      <c r="Y19" s="22"/>
-      <c r="Z19" s="22"/>
-    </row>
-    <row r="20" ht="72.0" customHeight="1">
-      <c r="B20" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="K20" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="M20" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="N20" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="O20" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="P20" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
-      <c r="T20" s="24"/>
-      <c r="U20" s="24"/>
-      <c r="V20" s="24"/>
-      <c r="W20" s="24"/>
-      <c r="X20" s="24"/>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="25"/>
-    </row>
-    <row r="21">
-      <c r="B21" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="27">
-        <v>36.0</v>
-      </c>
-      <c r="D21" s="27">
-        <v>41.0</v>
-      </c>
-      <c r="E21" s="27">
-        <v>38.0</v>
-      </c>
-      <c r="F21" s="27">
-        <v>29.0</v>
-      </c>
-      <c r="G21" s="27">
-        <v>36.0</v>
-      </c>
-      <c r="H21" s="27">
-        <v>41.0</v>
-      </c>
-      <c r="I21" s="27">
-        <v>40.0</v>
-      </c>
-      <c r="J21" s="27">
-        <v>37.0</v>
-      </c>
-      <c r="K21" s="27">
-        <v>38.0</v>
-      </c>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27">
-        <v>36.0</v>
-      </c>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27">
-        <v>31.0</v>
-      </c>
-      <c r="P21" s="27">
+      <c r="P20" s="27">
         <v>34.0</v>
       </c>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
-      <c r="V21" s="27"/>
-      <c r="W21" s="27"/>
-      <c r="X21" s="27"/>
-      <c r="Y21" s="27"/>
-      <c r="Z21" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1835,53 +1802,53 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>72</v>
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="4"/>
@@ -2014,7 +1981,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="12">
         <v>38.0</v>
@@ -2057,7 +2024,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
@@ -2151,7 +2118,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13">
@@ -2237,7 +2204,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C11" s="12">
         <v>33.0</v>
@@ -2278,7 +2245,7 @@
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -2319,7 +2286,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="12">
         <v>33.0</v>
@@ -2511,7 +2478,7 @@
     </row>
     <row r="17">
       <c r="B17" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="12">
         <v>31.0</v>
@@ -2560,7 +2527,7 @@
     </row>
     <row r="18">
       <c r="B18" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C18" s="12">
         <v>35.0</v>
@@ -2603,7 +2570,7 @@
     </row>
     <row r="19">
       <c r="B19" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C19" s="12">
         <v>33.0</v>
@@ -2656,7 +2623,7 @@
     </row>
     <row r="20">
       <c r="B20" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="12">
         <v>27.0</v>
@@ -2703,7 +2670,7 @@
     </row>
     <row r="21">
       <c r="B21" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="12">
         <v>31.0</v>
@@ -2748,7 +2715,7 @@
     </row>
     <row r="22">
       <c r="B22" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
@@ -2817,49 +2784,49 @@
     </row>
     <row r="24" ht="84.75" customHeight="1">
       <c r="B24" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="24" t="s">
         <v>73</v>
-      </c>
-      <c r="D24" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>74</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>48</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H24" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="I24" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="I24" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="J24" s="24" t="s">
+      <c r="K24" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="L24" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="K24" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="L24" s="24" t="s">
-        <v>85</v>
-      </c>
       <c r="M24" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N24" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O24" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P24" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Q24" s="24"/>
       <c r="R24" s="24"/>
@@ -2875,7 +2842,7 @@
     </row>
     <row r="25">
       <c r="B25" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="27">
         <v>38.0</v>
@@ -2950,15 +2917,15 @@
         <v>15</v>
       </c>
       <c r="B1" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="32" t="s">
         <v>86</v>
-      </c>
-      <c r="C1" s="32" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -2976,7 +2943,7 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -2985,7 +2952,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -2994,7 +2961,7 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -3003,7 +2970,7 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -3021,7 +2988,7 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -3030,7 +2997,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -3039,7 +3006,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -3075,7 +3042,7 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -3102,7 +3069,7 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="34">
@@ -3111,7 +3078,7 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="34">
@@ -3129,7 +3096,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="34">
@@ -3147,7 +3114,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="34">
@@ -3156,7 +3123,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="38">
@@ -7092,10 +7059,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3">
@@ -7103,10 +7070,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -7114,7 +7081,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="45" t="s">
         <v>44</v>
@@ -7128,7 +7095,7 @@
         <v>48</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6">
@@ -7139,7 +7106,7 @@
         <v>44</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7">
@@ -7147,7 +7114,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="45" t="s">
         <v>41</v>
@@ -7158,10 +7125,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9">
@@ -7169,7 +7136,7 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="45" t="s">
         <v>44</v>
@@ -7180,10 +7147,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7192,10 +7159,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12">
@@ -7203,10 +7170,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
@@ -7214,10 +7181,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14">
@@ -7225,10 +7192,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15">
@@ -7236,10 +7203,10 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
@@ -12217,11 +12184,11 @@
         <v>38</v>
       </c>
       <c r="D2" s="48" t="str">
+        <f>'THURSDAY SINGLES'!C19</f>
+        <v>JOHN ANTCLIFFE</v>
+      </c>
+      <c r="E2" s="47">
         <f>'THURSDAY SINGLES'!C20</f>
-        <v>JOHN ANTCLIFFE</v>
-      </c>
-      <c r="E2" s="47">
-        <f>'THURSDAY SINGLES'!C21</f>
         <v>36</v>
       </c>
     </row>
@@ -12238,11 +12205,11 @@
         <v>39</v>
       </c>
       <c r="D3" s="48" t="str">
+        <f>'THURSDAY SINGLES'!D19</f>
+        <v>MARTIN BROCK</v>
+      </c>
+      <c r="E3" s="47">
         <f>'THURSDAY SINGLES'!D20</f>
-        <v>MARTIN BROCK</v>
-      </c>
-      <c r="E3" s="47">
-        <f>'THURSDAY SINGLES'!D21</f>
         <v>41</v>
       </c>
     </row>
@@ -12259,11 +12226,11 @@
         <v>39</v>
       </c>
       <c r="D4" s="48" t="str">
+        <f>'THURSDAY SINGLES'!E19</f>
+        <v>STEW TAYLOR</v>
+      </c>
+      <c r="E4" s="47">
         <f>'THURSDAY SINGLES'!E20</f>
-        <v>STEW TAYLOR</v>
-      </c>
-      <c r="E4" s="47">
-        <f>'THURSDAY SINGLES'!E21</f>
         <v>38</v>
       </c>
     </row>
@@ -12280,11 +12247,11 @@
         <v>35</v>
       </c>
       <c r="D5" s="48" t="str">
+        <f>'THURSDAY SINGLES'!F19</f>
+        <v>KEN PEEL</v>
+      </c>
+      <c r="E5" s="47">
         <f>'THURSDAY SINGLES'!F20</f>
-        <v>KEN PEEL</v>
-      </c>
-      <c r="E5" s="47">
-        <f>'THURSDAY SINGLES'!F21</f>
         <v>29</v>
       </c>
     </row>
@@ -12301,11 +12268,11 @@
         <v>43</v>
       </c>
       <c r="D6" s="48" t="str">
+        <f>'THURSDAY SINGLES'!G19</f>
+        <v>LES DOBBINS</v>
+      </c>
+      <c r="E6" s="47">
         <f>'THURSDAY SINGLES'!G20</f>
-        <v>LES DOBBINS</v>
-      </c>
-      <c r="E6" s="47">
-        <f>'THURSDAY SINGLES'!G21</f>
         <v>36</v>
       </c>
     </row>
@@ -12322,11 +12289,11 @@
         <v>38</v>
       </c>
       <c r="D7" s="48" t="str">
+        <f>'THURSDAY SINGLES'!H19</f>
+        <v>MARTIN BROCK</v>
+      </c>
+      <c r="E7" s="47">
         <f>'THURSDAY SINGLES'!H20</f>
-        <v>MARTIN BROCK</v>
-      </c>
-      <c r="E7" s="47">
-        <f>'THURSDAY SINGLES'!H21</f>
         <v>41</v>
       </c>
     </row>
@@ -12343,11 +12310,11 @@
         <v>36</v>
       </c>
       <c r="D8" s="48" t="str">
-        <f>'THURSDAY SINGLES'!I20</f>
+        <f>'THURSDAY SINGLES'!I19</f>
         <v>DAVE BARNETT</v>
       </c>
       <c r="E8" s="47">
-        <f>'THURSDAY SINGLES'!I$21</f>
+        <f>'THURSDAY SINGLES'!I$20</f>
         <v>40</v>
       </c>
     </row>
@@ -12364,11 +12331,11 @@
         <v>35</v>
       </c>
       <c r="D9" s="48" t="str">
-        <f>'THURSDAY SINGLES'!J20</f>
+        <f>'THURSDAY SINGLES'!J19</f>
         <v>SCOTT LEONARDE</v>
       </c>
       <c r="E9" s="47">
-        <f>'THURSDAY SINGLES'!J$21</f>
+        <f>'THURSDAY SINGLES'!J$20</f>
         <v>37</v>
       </c>
     </row>
@@ -12385,11 +12352,11 @@
         <v>32</v>
       </c>
       <c r="D10" s="48" t="str">
-        <f>'THURSDAY SINGLES'!K20</f>
+        <f>'THURSDAY SINGLES'!K19</f>
         <v>ALBIE GILLESPIE</v>
       </c>
       <c r="E10" s="47">
-        <f>'THURSDAY SINGLES'!K$21</f>
+        <f>'THURSDAY SINGLES'!K$20</f>
         <v>38</v>
       </c>
     </row>
@@ -12406,11 +12373,11 @@
         <v>38</v>
       </c>
       <c r="D11" s="48" t="str">
-        <f>'THURSDAY SINGLES'!L20</f>
+        <f>'THURSDAY SINGLES'!L19</f>
         <v>N/A</v>
       </c>
       <c r="E11" s="47" t="str">
-        <f>'THURSDAY SINGLES'!L$21</f>
+        <f>'THURSDAY SINGLES'!L$20</f>
         <v/>
       </c>
     </row>
@@ -12427,11 +12394,11 @@
         <v>39</v>
       </c>
       <c r="D12" s="48" t="str">
+        <f>'THURSDAY SINGLES'!M19</f>
+        <v>TONY SLATER</v>
+      </c>
+      <c r="E12" s="47">
         <f>'THURSDAY SINGLES'!M20</f>
-        <v>TONY SLATER</v>
-      </c>
-      <c r="E12" s="47">
-        <f>'THURSDAY SINGLES'!M21</f>
         <v>36</v>
       </c>
     </row>
@@ -12448,11 +12415,11 @@
         <v/>
       </c>
       <c r="D13" s="48" t="str">
-        <f>'THURSDAY SINGLES'!N20</f>
+        <f>'THURSDAY SINGLES'!N19</f>
         <v>N/A</v>
       </c>
       <c r="E13" s="47" t="str">
-        <f>'THURSDAY SINGLES'!N$21</f>
+        <f>'THURSDAY SINGLES'!N$20</f>
         <v/>
       </c>
     </row>
@@ -12469,11 +12436,11 @@
         <v/>
       </c>
       <c r="D14" s="48" t="str">
+        <f>'THURSDAY SINGLES'!O19</f>
+        <v>LES DOBBINS</v>
+      </c>
+      <c r="E14" s="47">
         <f>'THURSDAY SINGLES'!O20</f>
-        <v>LES DOBBINS</v>
-      </c>
-      <c r="E14" s="47">
-        <f>'THURSDAY SINGLES'!O21</f>
         <v>31</v>
       </c>
     </row>
@@ -12490,11 +12457,11 @@
         <v/>
       </c>
       <c r="D15" s="48" t="str">
+        <f>'THURSDAY SINGLES'!P19</f>
+        <v>JODAN HOWARD</v>
+      </c>
+      <c r="E15" s="47">
         <f>'THURSDAY SINGLES'!P20</f>
-        <v>JODAN HOWARD</v>
-      </c>
-      <c r="E15" s="47">
-        <f>'THURSDAY SINGLES'!P21</f>
         <v>34</v>
       </c>
     </row>
@@ -12511,11 +12478,11 @@
         <v/>
       </c>
       <c r="D16" s="48" t="str">
+        <f>'THURSDAY SINGLES'!Q19</f>
+        <v/>
+      </c>
+      <c r="E16" s="47" t="str">
         <f>'THURSDAY SINGLES'!Q20</f>
-        <v/>
-      </c>
-      <c r="E16" s="47" t="str">
-        <f>'THURSDAY SINGLES'!Q21</f>
         <v/>
       </c>
     </row>
@@ -12532,11 +12499,11 @@
         <v/>
       </c>
       <c r="D17" s="48" t="str">
+        <f>'THURSDAY SINGLES'!R19</f>
+        <v/>
+      </c>
+      <c r="E17" s="47" t="str">
         <f>'THURSDAY SINGLES'!R20</f>
-        <v/>
-      </c>
-      <c r="E17" s="47" t="str">
-        <f>'THURSDAY SINGLES'!R21</f>
         <v/>
       </c>
     </row>
@@ -12553,11 +12520,11 @@
         <v/>
       </c>
       <c r="D18" s="48" t="str">
+        <f>'THURSDAY SINGLES'!S19</f>
+        <v/>
+      </c>
+      <c r="E18" s="47" t="str">
         <f>'THURSDAY SINGLES'!S20</f>
-        <v/>
-      </c>
-      <c r="E18" s="47" t="str">
-        <f>'THURSDAY SINGLES'!S21</f>
         <v/>
       </c>
     </row>
@@ -12574,11 +12541,11 @@
         <v/>
       </c>
       <c r="D19" s="48" t="str">
+        <f>'THURSDAY SINGLES'!T19</f>
+        <v/>
+      </c>
+      <c r="E19" s="47" t="str">
         <f>'THURSDAY SINGLES'!T20</f>
-        <v/>
-      </c>
-      <c r="E19" s="47" t="str">
-        <f>'THURSDAY SINGLES'!T21</f>
         <v/>
       </c>
     </row>
@@ -12595,11 +12562,11 @@
         <v/>
       </c>
       <c r="D20" s="48" t="str">
+        <f>'THURSDAY SINGLES'!U19</f>
+        <v/>
+      </c>
+      <c r="E20" s="47" t="str">
         <f>'THURSDAY SINGLES'!U20</f>
-        <v/>
-      </c>
-      <c r="E20" s="47" t="str">
-        <f>'THURSDAY SINGLES'!U21</f>
         <v/>
       </c>
     </row>
@@ -12616,11 +12583,11 @@
         <v/>
       </c>
       <c r="D21" s="48" t="str">
+        <f>'THURSDAY SINGLES'!V19</f>
+        <v/>
+      </c>
+      <c r="E21" s="47" t="str">
         <f>'THURSDAY SINGLES'!V20</f>
-        <v/>
-      </c>
-      <c r="E21" s="47" t="str">
-        <f>'THURSDAY SINGLES'!V21</f>
         <v/>
       </c>
     </row>
@@ -12637,11 +12604,11 @@
         <v/>
       </c>
       <c r="D22" s="48" t="str">
+        <f>'THURSDAY SINGLES'!W19</f>
+        <v/>
+      </c>
+      <c r="E22" s="47" t="str">
         <f>'THURSDAY SINGLES'!W20</f>
-        <v/>
-      </c>
-      <c r="E22" s="47" t="str">
-        <f>'THURSDAY SINGLES'!W21</f>
         <v/>
       </c>
     </row>
@@ -12658,11 +12625,11 @@
         <v/>
       </c>
       <c r="D23" s="48" t="str">
+        <f>'THURSDAY SINGLES'!X19</f>
+        <v/>
+      </c>
+      <c r="E23" s="47" t="str">
         <f>'THURSDAY SINGLES'!X20</f>
-        <v/>
-      </c>
-      <c r="E23" s="47" t="str">
-        <f>'THURSDAY SINGLES'!X21</f>
         <v/>
       </c>
     </row>
@@ -12679,11 +12646,11 @@
         <v/>
       </c>
       <c r="D24" s="48" t="str">
+        <f>'THURSDAY SINGLES'!Y19</f>
+        <v/>
+      </c>
+      <c r="E24" s="47" t="str">
         <f>'THURSDAY SINGLES'!Y20</f>
-        <v/>
-      </c>
-      <c r="E24" s="47" t="str">
-        <f>'THURSDAY SINGLES'!Y21</f>
         <v/>
       </c>
     </row>
@@ -12700,11 +12667,11 @@
         <v/>
       </c>
       <c r="D25" s="48" t="str">
+        <f>'THURSDAY SINGLES'!Z19</f>
+        <v/>
+      </c>
+      <c r="E25" s="47" t="str">
         <f>'THURSDAY SINGLES'!Z20</f>
-        <v/>
-      </c>
-      <c r="E25" s="47" t="str">
-        <f>'THURSDAY SINGLES'!Z21</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
084 Week 15/15 data update
</commit_message>
<xml_diff>
--- a/data/WINTER_GOLF_2526.xlsx
+++ b/data/WINTER_GOLF_2526.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="97">
   <si>
     <t>WINTER GOLF 25/26 - THURSDAY SINGLES</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>15th Jan 26</t>
+  </si>
+  <si>
+    <t>22nd Jan 26</t>
   </si>
   <si>
     <t>NAME</t>
@@ -231,6 +234,9 @@
   </si>
   <si>
     <t>18th Jan 26</t>
+  </si>
+  <si>
+    <t>25th Jan 26</t>
   </si>
   <si>
     <t>MICK SKINNER</t>
@@ -907,7 +913,9 @@
       <c r="P3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="R3" s="4"/>
       <c r="S3" s="3"/>
       <c r="T3" s="4"/>
@@ -921,87 +929,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13">
@@ -1054,7 +1062,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C6" s="12">
         <v>28.0</v>
@@ -1105,7 +1113,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="12">
         <v>31.0</v>
@@ -1135,7 +1143,9 @@
       <c r="P7" s="13">
         <v>33.0</v>
       </c>
-      <c r="Q7" s="15"/>
+      <c r="Q7" s="12">
+        <v>34.0</v>
+      </c>
       <c r="R7" s="13"/>
       <c r="S7" s="12"/>
       <c r="T7" s="13"/>
@@ -1147,12 +1157,12 @@
       <c r="Z7" s="18"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>239</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C8" s="12">
         <v>31.0</v>
@@ -1199,7 +1209,7 @@
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C9" s="12">
         <v>34.0</v>
@@ -1235,7 +1245,9 @@
       <c r="N9" s="13"/>
       <c r="O9" s="12"/>
       <c r="P9" s="13"/>
-      <c r="Q9" s="12"/>
+      <c r="Q9" s="12">
+        <v>34.0</v>
+      </c>
       <c r="R9" s="13"/>
       <c r="S9" s="12"/>
       <c r="T9" s="13"/>
@@ -1247,12 +1259,12 @@
       <c r="Z9" s="16"/>
       <c r="AA9" s="14">
         <f t="shared" si="1"/>
-        <v>298</v>
+        <v>332</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="12">
         <v>21.0</v>
@@ -1293,7 +1305,7 @@
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="12">
         <v>36.0</v>
@@ -1327,7 +1339,9 @@
         <v>24.0</v>
       </c>
       <c r="P11" s="14"/>
-      <c r="Q11" s="15"/>
+      <c r="Q11" s="12">
+        <v>29.0</v>
+      </c>
       <c r="R11" s="13"/>
       <c r="S11" s="12"/>
       <c r="T11" s="13"/>
@@ -1339,12 +1353,12 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>248</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="12">
         <v>35.0</v>
@@ -1395,7 +1409,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" s="12">
         <v>34.0</v>
@@ -1440,7 +1454,7 @@
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="12">
         <v>33.0</v>
@@ -1478,7 +1492,9 @@
       <c r="P14" s="13">
         <v>32.0</v>
       </c>
-      <c r="Q14" s="12"/>
+      <c r="Q14" s="12">
+        <v>37.0</v>
+      </c>
       <c r="R14" s="13"/>
       <c r="S14" s="12"/>
       <c r="T14" s="14"/>
@@ -1490,12 +1506,12 @@
       <c r="Z14" s="18"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>342</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="13"/>
@@ -1531,7 +1547,9 @@
       <c r="P15" s="13">
         <v>29.0</v>
       </c>
-      <c r="Q15" s="15"/>
+      <c r="Q15" s="12">
+        <v>26.0</v>
+      </c>
       <c r="R15" s="14"/>
       <c r="S15" s="12"/>
       <c r="T15" s="13"/>
@@ -1543,12 +1561,12 @@
       <c r="Z15" s="18"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>302</v>
+        <v>328</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="18">
         <v>26.0</v>
@@ -1578,7 +1596,9 @@
       <c r="P16" s="13">
         <v>34.0</v>
       </c>
-      <c r="Q16" s="15"/>
+      <c r="Q16" s="12">
+        <v>32.0</v>
+      </c>
       <c r="R16" s="13"/>
       <c r="S16" s="15"/>
       <c r="T16" s="13"/>
@@ -1590,12 +1610,12 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>213</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="21" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="12">
         <v>31.0</v>
@@ -1670,51 +1690,53 @@
     </row>
     <row r="19" ht="72.0" customHeight="1">
       <c r="B19" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="G19" s="24" t="s">
+      <c r="N19" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="O19" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="P19" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q19" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="H19" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="K19" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="L19" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="M19" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="N19" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="O19" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="P19" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
       <c r="S19" s="24"/>
       <c r="T19" s="24"/>
@@ -1728,7 +1750,7 @@
     </row>
     <row r="20">
       <c r="B20" s="26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="27">
         <v>36.0</v>
@@ -1768,7 +1790,9 @@
       <c r="P20" s="27">
         <v>34.0</v>
       </c>
-      <c r="Q20" s="27"/>
+      <c r="Q20" s="27">
+        <v>37.0</v>
+      </c>
       <c r="R20" s="27"/>
       <c r="S20" s="27"/>
       <c r="T20" s="27"/>
@@ -1802,55 +1826,57 @@
   <sheetData>
     <row r="2" ht="24.0" customHeight="1">
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="Z2" s="2"/>
       <c r="AA2" s="2"/>
     </row>
     <row r="3" ht="73.5" customHeight="1">
       <c r="C3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P3" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q3" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="R3" s="4"/>
       <c r="S3" s="3"/>
       <c r="T3" s="4"/>
@@ -1864,87 +1890,87 @@
     </row>
     <row r="4">
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X4" s="8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y4" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z4" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA4" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
@@ -1981,7 +2007,7 @@
     </row>
     <row r="6">
       <c r="B6" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C6" s="12">
         <v>38.0</v>
@@ -2024,7 +2050,7 @@
     </row>
     <row r="7">
       <c r="B7" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="13">
@@ -2058,7 +2084,9 @@
       <c r="N7" s="13"/>
       <c r="O7" s="15"/>
       <c r="P7" s="13"/>
-      <c r="Q7" s="12"/>
+      <c r="Q7" s="12">
+        <v>29.0</v>
+      </c>
       <c r="R7" s="13"/>
       <c r="S7" s="12"/>
       <c r="T7" s="13"/>
@@ -2070,12 +2098,12 @@
       <c r="Z7" s="16"/>
       <c r="AA7" s="14">
         <f t="shared" si="1"/>
-        <v>256</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="12">
         <v>28.0</v>
@@ -2101,7 +2129,9 @@
       <c r="N8" s="13"/>
       <c r="O8" s="12"/>
       <c r="P8" s="13"/>
-      <c r="Q8" s="12"/>
+      <c r="Q8" s="12">
+        <v>34.0</v>
+      </c>
       <c r="R8" s="13"/>
       <c r="S8" s="12"/>
       <c r="T8" s="14"/>
@@ -2113,12 +2143,12 @@
       <c r="Z8" s="18"/>
       <c r="AA8" s="14">
         <f t="shared" si="1"/>
-        <v>147</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="13">
@@ -2161,7 +2191,7 @@
     </row>
     <row r="10">
       <c r="B10" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="13"/>
@@ -2187,7 +2217,9 @@
       <c r="N10" s="13"/>
       <c r="O10" s="12"/>
       <c r="P10" s="14"/>
-      <c r="Q10" s="12"/>
+      <c r="Q10" s="12">
+        <v>27.0</v>
+      </c>
       <c r="R10" s="13"/>
       <c r="S10" s="15"/>
       <c r="T10" s="13"/>
@@ -2199,12 +2231,12 @@
       <c r="Z10" s="16"/>
       <c r="AA10" s="14">
         <f t="shared" si="1"/>
-        <v>167</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C11" s="12">
         <v>33.0</v>
@@ -2228,7 +2260,9 @@
       <c r="N11" s="14"/>
       <c r="O11" s="12"/>
       <c r="P11" s="13"/>
-      <c r="Q11" s="15"/>
+      <c r="Q11" s="12">
+        <v>34.0</v>
+      </c>
       <c r="R11" s="14"/>
       <c r="S11" s="15"/>
       <c r="T11" s="14"/>
@@ -2240,12 +2274,12 @@
       <c r="Z11" s="16"/>
       <c r="AA11" s="14">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="17" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="13"/>
@@ -2286,7 +2320,7 @@
     </row>
     <row r="13">
       <c r="B13" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C13" s="12">
         <v>33.0</v>
@@ -2316,7 +2350,9 @@
       <c r="N13" s="13"/>
       <c r="O13" s="12"/>
       <c r="P13" s="14"/>
-      <c r="Q13" s="15"/>
+      <c r="Q13" s="12">
+        <v>25.0</v>
+      </c>
       <c r="R13" s="14"/>
       <c r="S13" s="15"/>
       <c r="T13" s="13"/>
@@ -2328,12 +2364,12 @@
       <c r="Z13" s="16"/>
       <c r="AA13" s="14">
         <f t="shared" si="1"/>
-        <v>210</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C14" s="12">
         <v>29.0</v>
@@ -2367,7 +2403,9 @@
       <c r="N14" s="13"/>
       <c r="O14" s="12"/>
       <c r="P14" s="13"/>
-      <c r="Q14" s="12"/>
+      <c r="Q14" s="12">
+        <v>26.0</v>
+      </c>
       <c r="R14" s="14"/>
       <c r="S14" s="15"/>
       <c r="T14" s="14"/>
@@ -2379,12 +2417,12 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="14">
         <f t="shared" si="1"/>
-        <v>263</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="12">
         <v>28.0</v>
@@ -2416,7 +2454,9 @@
       <c r="N15" s="14"/>
       <c r="O15" s="15"/>
       <c r="P15" s="14"/>
-      <c r="Q15" s="12"/>
+      <c r="Q15" s="12">
+        <v>34.0</v>
+      </c>
       <c r="R15" s="14"/>
       <c r="S15" s="12"/>
       <c r="T15" s="14"/>
@@ -2428,12 +2468,12 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="14">
         <f t="shared" si="1"/>
-        <v>233</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C16" s="12">
         <v>24.0</v>
@@ -2461,7 +2501,9 @@
       <c r="N16" s="13"/>
       <c r="O16" s="12"/>
       <c r="P16" s="13"/>
-      <c r="Q16" s="12"/>
+      <c r="Q16" s="12">
+        <v>32.0</v>
+      </c>
       <c r="R16" s="14"/>
       <c r="S16" s="12"/>
       <c r="T16" s="14"/>
@@ -2473,12 +2515,12 @@
       <c r="Z16" s="16"/>
       <c r="AA16" s="14">
         <f t="shared" si="1"/>
-        <v>186</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C17" s="12">
         <v>31.0</v>
@@ -2510,7 +2552,9 @@
       <c r="N17" s="13"/>
       <c r="O17" s="12"/>
       <c r="P17" s="14"/>
-      <c r="Q17" s="12"/>
+      <c r="Q17" s="12">
+        <v>31.0</v>
+      </c>
       <c r="R17" s="14"/>
       <c r="S17" s="12"/>
       <c r="T17" s="13"/>
@@ -2522,12 +2566,12 @@
       <c r="Z17" s="16"/>
       <c r="AA17" s="14">
         <f t="shared" si="1"/>
-        <v>250</v>
+        <v>281</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C18" s="12">
         <v>35.0</v>
@@ -2553,7 +2597,9 @@
       <c r="N18" s="13"/>
       <c r="O18" s="12"/>
       <c r="P18" s="13"/>
-      <c r="Q18" s="15"/>
+      <c r="Q18" s="12">
+        <v>33.0</v>
+      </c>
       <c r="R18" s="14"/>
       <c r="S18" s="15"/>
       <c r="T18" s="13"/>
@@ -2565,12 +2611,12 @@
       <c r="Z18" s="18"/>
       <c r="AA18" s="14">
         <f t="shared" si="1"/>
-        <v>163</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C19" s="12">
         <v>33.0</v>
@@ -2606,7 +2652,9 @@
       <c r="N19" s="14"/>
       <c r="O19" s="15"/>
       <c r="P19" s="14"/>
-      <c r="Q19" s="15"/>
+      <c r="Q19" s="12">
+        <v>28.0</v>
+      </c>
       <c r="R19" s="14"/>
       <c r="S19" s="12"/>
       <c r="T19" s="14"/>
@@ -2618,12 +2666,12 @@
       <c r="Z19" s="16"/>
       <c r="AA19" s="14">
         <f t="shared" si="1"/>
-        <v>326</v>
+        <v>354</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="17" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C20" s="12">
         <v>27.0</v>
@@ -2653,7 +2701,9 @@
       <c r="N20" s="13"/>
       <c r="O20" s="12"/>
       <c r="P20" s="14"/>
-      <c r="Q20" s="12"/>
+      <c r="Q20" s="12">
+        <v>31.0</v>
+      </c>
       <c r="R20" s="14"/>
       <c r="S20" s="12"/>
       <c r="T20" s="13"/>
@@ -2665,12 +2715,12 @@
       <c r="Z20" s="18"/>
       <c r="AA20" s="14">
         <f t="shared" si="1"/>
-        <v>202</v>
+        <v>233</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="17" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C21" s="12">
         <v>31.0</v>
@@ -2715,7 +2765,7 @@
     </row>
     <row r="22">
       <c r="B22" s="28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
@@ -2784,51 +2834,53 @@
     </row>
     <row r="24" ht="84.75" customHeight="1">
       <c r="B24" s="23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" s="24" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E24" s="24" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="L24" s="24" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="N24" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="O24" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="P24" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q24" s="24"/>
+        <v>56</v>
+      </c>
+      <c r="Q24" s="24" t="s">
+        <v>86</v>
+      </c>
       <c r="R24" s="24"/>
       <c r="S24" s="24"/>
       <c r="T24" s="24"/>
@@ -2842,7 +2894,7 @@
     </row>
     <row r="25">
       <c r="B25" s="26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C25" s="27">
         <v>38.0</v>
@@ -2880,7 +2932,9 @@
       <c r="N25" s="27"/>
       <c r="O25" s="27"/>
       <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
+      <c r="Q25" s="27">
+        <v>36.0</v>
+      </c>
       <c r="R25" s="27"/>
       <c r="S25" s="27"/>
       <c r="T25" s="27"/>
@@ -2914,18 +2968,18 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B2" s="33"/>
       <c r="C2" s="34">
@@ -2934,7 +2988,7 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="34">
@@ -2943,7 +2997,7 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B4" s="33"/>
       <c r="C4" s="34">
@@ -2952,7 +3006,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B5" s="33"/>
       <c r="C5" s="34">
@@ -2961,7 +3015,7 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B6" s="33"/>
       <c r="C6" s="34">
@@ -2970,7 +3024,7 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B7" s="33"/>
       <c r="C7" s="34">
@@ -2979,7 +3033,7 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="33"/>
       <c r="C8" s="34">
@@ -2988,7 +3042,7 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B9" s="33"/>
       <c r="C9" s="34">
@@ -2997,7 +3051,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B10" s="33"/>
       <c r="C10" s="34">
@@ -3006,7 +3060,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B11" s="33"/>
       <c r="C11" s="34">
@@ -3015,7 +3069,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="35">
@@ -3024,7 +3078,7 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34">
@@ -3033,7 +3087,7 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34">
@@ -3042,7 +3096,7 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="33"/>
       <c r="C15" s="34">
@@ -3051,7 +3105,7 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="33"/>
       <c r="C16" s="34">
@@ -3060,7 +3114,7 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="33"/>
       <c r="C17" s="34">
@@ -3069,7 +3123,7 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B18" s="33"/>
       <c r="C18" s="34">
@@ -3078,7 +3132,7 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B19" s="33"/>
       <c r="C19" s="34">
@@ -3087,7 +3141,7 @@
     </row>
     <row r="20">
       <c r="A20" s="36" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B20" s="33"/>
       <c r="C20" s="34">
@@ -3096,7 +3150,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B21" s="33"/>
       <c r="C21" s="34">
@@ -3105,7 +3159,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22" s="33"/>
       <c r="C22" s="34">
@@ -3114,7 +3168,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B23" s="33"/>
       <c r="C23" s="34">
@@ -3123,7 +3177,7 @@
     </row>
     <row r="24">
       <c r="A24" s="28" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B24" s="37"/>
       <c r="C24" s="38">
@@ -3132,7 +3186,7 @@
     </row>
     <row r="25">
       <c r="A25" s="36" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" s="14"/>
       <c r="C25" s="13">
@@ -7045,13 +7099,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C1" s="40" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2">
@@ -7059,10 +7113,10 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C2" s="43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
@@ -7070,10 +7124,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C3" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4">
@@ -7081,10 +7135,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="44" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C4" s="45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5">
@@ -7092,10 +7146,10 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C5" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6">
@@ -7103,10 +7157,10 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="44" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C6" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7">
@@ -7114,10 +7168,10 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="44" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C7" s="45" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8">
@@ -7125,10 +7179,10 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9">
@@ -7136,10 +7190,10 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="44" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10">
@@ -7147,10 +7201,10 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G10" s="14"/>
     </row>
@@ -7159,10 +7213,10 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
@@ -7170,10 +7224,10 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -7181,10 +7235,10 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -7192,10 +7246,10 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15">
@@ -7203,18 +7257,22 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="44" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="13">
         <v>15.0</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="45"/>
+      <c r="B16" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="13">
@@ -12156,19 +12214,19 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2">
@@ -12471,19 +12529,19 @@
       </c>
       <c r="B16" s="47" t="str">
         <f>'SUNDAY SINGLES'!Q24</f>
-        <v/>
-      </c>
-      <c r="C16" s="47" t="str">
+        <v>PAUL HANCOX</v>
+      </c>
+      <c r="C16" s="47">
         <f>'SUNDAY SINGLES'!Q25</f>
-        <v/>
+        <v>36</v>
       </c>
       <c r="D16" s="48" t="str">
         <f>'THURSDAY SINGLES'!Q19</f>
-        <v/>
-      </c>
-      <c r="E16" s="47" t="str">
+        <v>ALBIE GILLESPIE</v>
+      </c>
+      <c r="E16" s="47">
         <f>'THURSDAY SINGLES'!Q20</f>
-        <v/>
+        <v>37</v>
       </c>
     </row>
     <row r="17">

</xml_diff>